<commit_message>
Add atempt to found equations for soles
</commit_message>
<xml_diff>
--- a/static/mock/titanium sols.xlsx
+++ b/static/mock/titanium sols.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexglushko/PycharmProjects/ChemML/static/mock/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0054548-138E-B347-BD41-3053EC144914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354F1F54-9F69-734F-A69C-C06DBE12F2DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{DA8300D2-1843-2443-8DD6-A95A819FF1FD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{DA8300D2-1843-2443-8DD6-A95A819FF1FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="150">
   <si>
     <t>Состав реакционных смесей</t>
   </si>
@@ -889,9 +889,6 @@
   </si>
   <si>
     <t>75</t>
-  </si>
-  <si>
-    <t>100,0</t>
   </si>
   <si>
     <t>2000</t>
@@ -1181,7 +1178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1210,25 +1207,22 @@
     <xf numFmtId="16" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1261,32 +1255,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1294,28 +1287,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1479,6 +1450,28 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1493,18 +1486,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5DF1502E-028D-1344-AE85-5B77C048C3F1}" name="Table1" displayName="Table1" ref="A1:I72" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5DF1502E-028D-1344-AE85-5B77C048C3F1}" name="Table1" displayName="Table1" ref="A1:I72" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:I72" xr:uid="{5DF1502E-028D-1344-AE85-5B77C048C3F1}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{3D730327-C2DB-9E4A-80C1-BAFAA7500357}" name="Composition mixtures" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{F82AE513-B717-6747-9287-CEBC5038457A}" name="t, °С" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{9F227F16-6DE9-CA4F-BFE3-4F60F03ED1A4}" name="t, min" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{1799F322-44C3-E444-BB63-1C5EE13CA093}" name="с(acid), mol/l" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{2CA3ADB1-9B11-E846-B0C3-0E7782922E73}" name="с(Ti4+), mol/l" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{B2897B7A-1D41-1B44-8874-0A91AC14F034}" name="ultrasound " dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{1F319DDF-3186-4140-91A3-60695E430856}" name="d, nm" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{E5061E4A-695A-4149-B33A-FBEA0206A69B}" name="Contents, %" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{79A7B4D1-F871-374F-91F9-E3469D6727B7}" name="Stability of sols, days" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{3D730327-C2DB-9E4A-80C1-BAFAA7500357}" name="Composition mixtures" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{F82AE513-B717-6747-9287-CEBC5038457A}" name="t, °С" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{9F227F16-6DE9-CA4F-BFE3-4F60F03ED1A4}" name="t, min" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{1799F322-44C3-E444-BB63-1C5EE13CA093}" name="с(acid), mol/l" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{2CA3ADB1-9B11-E846-B0C3-0E7782922E73}" name="с(Ti4+), mol/l" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{B2897B7A-1D41-1B44-8874-0A91AC14F034}" name="ultrasound " dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{1F319DDF-3186-4140-91A3-60695E430856}" name="d, nm" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{E5061E4A-695A-4149-B33A-FBEA0206A69B}" name="Contents, %" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{79A7B4D1-F871-374F-91F9-E3469D6727B7}" name="Stability of sols, days" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1816,67 +1809,67 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="24"/>
-      <c r="I1" s="17" t="s">
+      <c r="H1" s="23"/>
+      <c r="I1" s="16" t="s">
         <v>3</v>
       </c>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="13" t="s">
+      <c r="A2" s="17"/>
+      <c r="B2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="28" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="18"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="17"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="28"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="29"/>
       <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
       <c r="G3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="19"/>
+      <c r="I3" s="18"/>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="26" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="3">
@@ -1906,7 +1899,7 @@
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="A5" s="31"/>
       <c r="B5" s="3">
         <v>80</v>
       </c>
@@ -1934,7 +1927,7 @@
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="3">
         <v>45</v>
       </c>
@@ -1962,7 +1955,7 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="3">
         <v>45</v>
       </c>
@@ -1990,7 +1983,7 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="26" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="3">
@@ -2020,7 +2013,7 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="3">
         <v>50</v>
       </c>
@@ -2048,7 +2041,7 @@
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="3">
         <v>80</v>
       </c>
@@ -2076,7 +2069,7 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="3">
         <v>45</v>
       </c>
@@ -2104,7 +2097,7 @@
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="3">
         <v>60</v>
       </c>
@@ -2132,7 +2125,7 @@
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
+      <c r="A13" s="31"/>
       <c r="B13" s="3">
         <v>60</v>
       </c>
@@ -2160,20 +2153,20 @@
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="16"/>
-      <c r="B14" s="13">
+      <c r="A14" s="31"/>
+      <c r="B14" s="26">
         <v>45</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="26">
         <v>130</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="13" t="s">
+      <c r="D14" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="26" t="s">
         <v>14</v>
       </c>
       <c r="G14" s="6">
@@ -2182,29 +2175,29 @@
       <c r="H14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="26">
         <v>9</v>
       </c>
-      <c r="J14" s="15"/>
+      <c r="J14" s="30"/>
     </row>
     <row r="15" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
       <c r="G15" s="5">
         <v>45006</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="14"/>
-      <c r="J15" s="15"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="30"/>
     </row>
     <row r="16" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="3">
         <v>45</v>
       </c>
@@ -2232,7 +2225,7 @@
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
+      <c r="A17" s="31"/>
       <c r="B17" s="3">
         <v>25</v>
       </c>
@@ -2260,7 +2253,7 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
+      <c r="A18" s="31"/>
       <c r="B18" s="3">
         <v>45</v>
       </c>
@@ -2288,7 +2281,7 @@
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="3">
         <v>25</v>
       </c>
@@ -2316,7 +2309,7 @@
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
+      <c r="A20" s="31"/>
       <c r="B20" s="3">
         <v>20</v>
       </c>
@@ -2344,7 +2337,7 @@
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
+      <c r="A21" s="31"/>
       <c r="B21" s="3">
         <v>80</v>
       </c>
@@ -2372,7 +2365,7 @@
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="3">
         <v>45</v>
       </c>
@@ -2400,22 +2393,22 @@
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="13">
+      <c r="B23" s="26">
         <v>50</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="26">
         <v>30</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="26">
         <v>4</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="13" t="s">
+      <c r="F23" s="26" t="s">
         <v>14</v>
       </c>
       <c r="G23" s="2">
@@ -2424,29 +2417,29 @@
       <c r="H23" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I23" s="13">
+      <c r="I23" s="26">
         <v>17</v>
       </c>
-      <c r="J23" s="15"/>
+      <c r="J23" s="30"/>
     </row>
     <row r="24" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
       <c r="G24" s="3" t="s">
         <v>35</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I24" s="14"/>
-      <c r="J24" s="15"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="30"/>
     </row>
     <row r="25" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
+      <c r="A25" s="31"/>
       <c r="B25" s="3">
         <v>80</v>
       </c>
@@ -2474,7 +2467,7 @@
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
+      <c r="A26" s="31"/>
       <c r="B26" s="3">
         <v>45</v>
       </c>
@@ -2502,7 +2495,7 @@
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
+      <c r="A27" s="31"/>
       <c r="B27" s="3">
         <v>60</v>
       </c>
@@ -2530,7 +2523,7 @@
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
+      <c r="A28" s="31"/>
       <c r="B28" s="3">
         <v>60</v>
       </c>
@@ -2558,7 +2551,7 @@
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
+      <c r="A29" s="31"/>
       <c r="B29" s="3">
         <v>60</v>
       </c>
@@ -2586,7 +2579,7 @@
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
+      <c r="A30" s="31"/>
       <c r="B30" s="3">
         <v>80</v>
       </c>
@@ -2614,7 +2607,7 @@
       <c r="J30" s="1"/>
     </row>
     <row r="31" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
+      <c r="A31" s="31"/>
       <c r="B31" s="3">
         <v>60</v>
       </c>
@@ -2642,7 +2635,7 @@
       <c r="J31" s="1"/>
     </row>
     <row r="32" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
+      <c r="A32" s="31"/>
       <c r="B32" s="3">
         <v>45</v>
       </c>
@@ -2670,7 +2663,7 @@
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
+      <c r="A33" s="31"/>
       <c r="B33" s="3">
         <v>20</v>
       </c>
@@ -2698,7 +2691,7 @@
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
+      <c r="A34" s="31"/>
       <c r="B34" s="3">
         <v>20</v>
       </c>
@@ -2726,7 +2719,7 @@
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
+      <c r="A35" s="31"/>
       <c r="B35" s="3">
         <v>20</v>
       </c>
@@ -2754,7 +2747,7 @@
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="16"/>
+      <c r="A36" s="31"/>
       <c r="B36" s="3">
         <v>25</v>
       </c>
@@ -2782,7 +2775,7 @@
       <c r="J36" s="1"/>
     </row>
     <row r="37" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="16"/>
+      <c r="A37" s="31"/>
       <c r="B37" s="3">
         <v>45</v>
       </c>
@@ -2810,7 +2803,7 @@
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
+      <c r="A38" s="27"/>
       <c r="B38" s="3">
         <v>45</v>
       </c>
@@ -2838,7 +2831,7 @@
       <c r="J38" s="1"/>
     </row>
     <row r="39" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B39" s="3">
@@ -2868,7 +2861,7 @@
       <c r="J39" s="1"/>
     </row>
     <row r="40" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="16"/>
+      <c r="A40" s="31"/>
       <c r="B40" s="8">
         <v>80</v>
       </c>
@@ -2896,7 +2889,7 @@
       <c r="J40" s="1"/>
     </row>
     <row r="41" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="16"/>
+      <c r="A41" s="31"/>
       <c r="B41" s="8">
         <v>80</v>
       </c>
@@ -2924,7 +2917,7 @@
       <c r="J41" s="1"/>
     </row>
     <row r="42" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="16"/>
+      <c r="A42" s="31"/>
       <c r="B42" s="8">
         <v>80</v>
       </c>
@@ -2952,7 +2945,7 @@
       <c r="J42" s="1"/>
     </row>
     <row r="43" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="16"/>
+      <c r="A43" s="31"/>
       <c r="B43" s="8">
         <v>80</v>
       </c>
@@ -2980,7 +2973,7 @@
       <c r="J43" s="1"/>
     </row>
     <row r="44" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="16"/>
+      <c r="A44" s="31"/>
       <c r="B44" s="8">
         <v>85</v>
       </c>
@@ -3008,7 +3001,7 @@
       <c r="J44" s="1"/>
     </row>
     <row r="45" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="16"/>
+      <c r="A45" s="31"/>
       <c r="B45" s="8">
         <v>88</v>
       </c>
@@ -3036,7 +3029,7 @@
       <c r="J45" s="1"/>
     </row>
     <row r="46" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="16"/>
+      <c r="A46" s="31"/>
       <c r="B46" s="8">
         <v>88</v>
       </c>
@@ -3064,7 +3057,7 @@
       <c r="J46" s="1"/>
     </row>
     <row r="47" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="16"/>
+      <c r="A47" s="31"/>
       <c r="B47" s="8">
         <v>89</v>
       </c>
@@ -3092,7 +3085,7 @@
       <c r="J47" s="1"/>
     </row>
     <row r="48" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="16"/>
+      <c r="A48" s="31"/>
       <c r="B48" s="8">
         <v>89</v>
       </c>
@@ -3120,7 +3113,7 @@
       <c r="J48" s="1"/>
     </row>
     <row r="49" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="16"/>
+      <c r="A49" s="31"/>
       <c r="B49" s="8">
         <v>93</v>
       </c>
@@ -3148,7 +3141,7 @@
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="16"/>
+      <c r="A50" s="31"/>
       <c r="B50" s="8">
         <v>93</v>
       </c>
@@ -3176,17 +3169,17 @@
       <c r="J50" s="1"/>
     </row>
     <row r="51" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="16"/>
-      <c r="B51" s="10">
+      <c r="A51" s="31"/>
+      <c r="B51" s="32">
         <v>71</v>
       </c>
-      <c r="C51" s="10">
+      <c r="C51" s="32">
         <v>9</v>
       </c>
-      <c r="D51" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E51" s="10" t="s">
+      <c r="D51" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" s="32" t="s">
         <v>44</v>
       </c>
       <c r="F51" s="8" t="s">
@@ -3204,11 +3197,11 @@
       <c r="J51" s="1"/>
     </row>
     <row r="52" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="16"/>
-      <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
+      <c r="A52" s="31"/>
+      <c r="B52" s="33"/>
+      <c r="C52" s="33"/>
+      <c r="D52" s="33"/>
+      <c r="E52" s="33"/>
       <c r="F52" s="8" t="s">
         <v>13</v>
       </c>
@@ -3224,11 +3217,11 @@
       <c r="J52" s="1"/>
     </row>
     <row r="53" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="16"/>
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="11"/>
+      <c r="A53" s="31"/>
+      <c r="B53" s="33"/>
+      <c r="C53" s="33"/>
+      <c r="D53" s="33"/>
+      <c r="E53" s="33"/>
       <c r="F53" s="8">
         <v>1</v>
       </c>
@@ -3244,11 +3237,11 @@
       <c r="J53" s="1"/>
     </row>
     <row r="54" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="16"/>
-      <c r="B54" s="12"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
+      <c r="A54" s="31"/>
+      <c r="B54" s="34"/>
+      <c r="C54" s="34"/>
+      <c r="D54" s="34"/>
+      <c r="E54" s="34"/>
       <c r="F54" s="9">
         <v>45047</v>
       </c>
@@ -3264,17 +3257,17 @@
       <c r="J54" s="1"/>
     </row>
     <row r="55" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="16"/>
-      <c r="B55" s="10">
+      <c r="A55" s="31"/>
+      <c r="B55" s="32">
         <v>71</v>
       </c>
-      <c r="C55" s="10">
+      <c r="C55" s="32">
         <v>10</v>
       </c>
-      <c r="D55" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E55" s="10" t="s">
+      <c r="D55" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="E55" s="32" t="s">
         <v>44</v>
       </c>
       <c r="F55" s="8" t="s">
@@ -3292,11 +3285,11 @@
       <c r="J55" s="1"/>
     </row>
     <row r="56" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="16"/>
-      <c r="B56" s="11"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="11"/>
-      <c r="E56" s="11"/>
+      <c r="A56" s="31"/>
+      <c r="B56" s="33"/>
+      <c r="C56" s="33"/>
+      <c r="D56" s="33"/>
+      <c r="E56" s="33"/>
       <c r="F56" s="8" t="s">
         <v>13</v>
       </c>
@@ -3312,11 +3305,11 @@
       <c r="J56" s="1"/>
     </row>
     <row r="57" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="16"/>
-      <c r="B57" s="11"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11"/>
+      <c r="A57" s="31"/>
+      <c r="B57" s="33"/>
+      <c r="C57" s="33"/>
+      <c r="D57" s="33"/>
+      <c r="E57" s="33"/>
       <c r="F57" s="8">
         <v>1</v>
       </c>
@@ -3332,11 +3325,11 @@
       <c r="J57" s="1"/>
     </row>
     <row r="58" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="16"/>
-      <c r="B58" s="12"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="12"/>
+      <c r="A58" s="31"/>
+      <c r="B58" s="34"/>
+      <c r="C58" s="34"/>
+      <c r="D58" s="34"/>
+      <c r="E58" s="34"/>
       <c r="F58" s="9">
         <v>45047</v>
       </c>
@@ -3352,17 +3345,17 @@
       <c r="J58" s="1"/>
     </row>
     <row r="59" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="16"/>
-      <c r="B59" s="10">
+      <c r="A59" s="31"/>
+      <c r="B59" s="32">
         <v>71</v>
       </c>
-      <c r="C59" s="10">
+      <c r="C59" s="32">
         <v>11</v>
       </c>
-      <c r="D59" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E59" s="10" t="s">
+      <c r="D59" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="E59" s="32" t="s">
         <v>44</v>
       </c>
       <c r="F59" s="8" t="s">
@@ -3380,11 +3373,11 @@
       <c r="J59" s="1"/>
     </row>
     <row r="60" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="16"/>
-      <c r="B60" s="11"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="11"/>
+      <c r="A60" s="31"/>
+      <c r="B60" s="33"/>
+      <c r="C60" s="33"/>
+      <c r="D60" s="33"/>
+      <c r="E60" s="33"/>
       <c r="F60" s="8" t="s">
         <v>13</v>
       </c>
@@ -3400,11 +3393,11 @@
       <c r="J60" s="1"/>
     </row>
     <row r="61" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="16"/>
-      <c r="B61" s="11"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
+      <c r="A61" s="31"/>
+      <c r="B61" s="33"/>
+      <c r="C61" s="33"/>
+      <c r="D61" s="33"/>
+      <c r="E61" s="33"/>
       <c r="F61" s="8">
         <v>1</v>
       </c>
@@ -3420,11 +3413,11 @@
       <c r="J61" s="1"/>
     </row>
     <row r="62" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="16"/>
-      <c r="B62" s="12"/>
-      <c r="C62" s="12"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="12"/>
+      <c r="A62" s="31"/>
+      <c r="B62" s="34"/>
+      <c r="C62" s="34"/>
+      <c r="D62" s="34"/>
+      <c r="E62" s="34"/>
       <c r="F62" s="9">
         <v>45047</v>
       </c>
@@ -3440,17 +3433,17 @@
       <c r="J62" s="1"/>
     </row>
     <row r="63" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="16"/>
-      <c r="B63" s="10">
+      <c r="A63" s="31"/>
+      <c r="B63" s="32">
         <v>71</v>
       </c>
-      <c r="C63" s="10">
+      <c r="C63" s="32">
         <v>12</v>
       </c>
-      <c r="D63" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E63" s="10" t="s">
+      <c r="D63" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="E63" s="32" t="s">
         <v>44</v>
       </c>
       <c r="F63" s="8" t="s">
@@ -3468,11 +3461,11 @@
       <c r="J63" s="1"/>
     </row>
     <row r="64" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="16"/>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="11"/>
+      <c r="A64" s="31"/>
+      <c r="B64" s="33"/>
+      <c r="C64" s="33"/>
+      <c r="D64" s="33"/>
+      <c r="E64" s="33"/>
       <c r="F64" s="8" t="s">
         <v>13</v>
       </c>
@@ -3488,11 +3481,11 @@
       <c r="J64" s="1"/>
     </row>
     <row r="65" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="16"/>
-      <c r="B65" s="11"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="11"/>
-      <c r="E65" s="11"/>
+      <c r="A65" s="31"/>
+      <c r="B65" s="33"/>
+      <c r="C65" s="33"/>
+      <c r="D65" s="33"/>
+      <c r="E65" s="33"/>
       <c r="F65" s="8">
         <v>1</v>
       </c>
@@ -3508,11 +3501,11 @@
       <c r="J65" s="1"/>
     </row>
     <row r="66" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="16"/>
-      <c r="B66" s="12"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="12"/>
-      <c r="E66" s="12"/>
+      <c r="A66" s="31"/>
+      <c r="B66" s="34"/>
+      <c r="C66" s="34"/>
+      <c r="D66" s="34"/>
+      <c r="E66" s="34"/>
       <c r="F66" s="9">
         <v>45047</v>
       </c>
@@ -3528,7 +3521,7 @@
       <c r="J66" s="1"/>
     </row>
     <row r="67" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="16"/>
+      <c r="A67" s="31"/>
       <c r="B67" s="8">
         <v>65</v>
       </c>
@@ -3556,7 +3549,7 @@
       <c r="J67" s="1"/>
     </row>
     <row r="68" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="16"/>
+      <c r="A68" s="31"/>
       <c r="B68" s="8">
         <v>75</v>
       </c>
@@ -3584,7 +3577,7 @@
       <c r="J68" s="1"/>
     </row>
     <row r="69" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="16"/>
+      <c r="A69" s="31"/>
       <c r="B69" s="8">
         <v>85</v>
       </c>
@@ -3612,7 +3605,7 @@
       <c r="J69" s="1"/>
     </row>
     <row r="70" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="16"/>
+      <c r="A70" s="31"/>
       <c r="B70" s="8">
         <v>70</v>
       </c>
@@ -3640,7 +3633,7 @@
       <c r="J70" s="1"/>
     </row>
     <row r="71" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="16"/>
+      <c r="A71" s="31"/>
       <c r="B71" s="8">
         <v>70</v>
       </c>
@@ -3668,7 +3661,7 @@
       <c r="J71" s="1"/>
     </row>
     <row r="72" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="16"/>
+      <c r="A72" s="31"/>
       <c r="B72" s="8">
         <v>70</v>
       </c>
@@ -3696,7 +3689,7 @@
       <c r="J72" s="1"/>
     </row>
     <row r="73" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="16"/>
+      <c r="A73" s="31"/>
       <c r="B73" s="8">
         <v>70</v>
       </c>
@@ -3724,7 +3717,7 @@
       <c r="J73" s="1"/>
     </row>
     <row r="74" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="14"/>
+      <c r="A74" s="27"/>
       <c r="B74" s="8">
         <v>80</v>
       </c>
@@ -3753,22 +3746,15 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="G1:H2"/>
-    <mergeCell ref="I1:I3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="A23:A38"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A22"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="D63:D66"/>
+    <mergeCell ref="E63:E66"/>
+    <mergeCell ref="E55:E58"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="C59:C62"/>
+    <mergeCell ref="D59:D62"/>
+    <mergeCell ref="E59:E62"/>
     <mergeCell ref="A39:A74"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:E15"/>
@@ -3778,7 +3764,6 @@
     <mergeCell ref="E23:E24"/>
     <mergeCell ref="F23:F24"/>
     <mergeCell ref="I23:I24"/>
-    <mergeCell ref="J23:J24"/>
     <mergeCell ref="B51:B54"/>
     <mergeCell ref="C51:C54"/>
     <mergeCell ref="D51:D54"/>
@@ -3786,15 +3771,23 @@
     <mergeCell ref="B55:B58"/>
     <mergeCell ref="C55:C58"/>
     <mergeCell ref="D55:D58"/>
-    <mergeCell ref="E55:E58"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="C59:C62"/>
-    <mergeCell ref="D59:D62"/>
-    <mergeCell ref="E59:E62"/>
-    <mergeCell ref="B63:B66"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="D63:D66"/>
-    <mergeCell ref="E63:E66"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="A23:A38"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A22"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:H2"/>
+    <mergeCell ref="I1:I3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3805,7 +3798,7 @@
   <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="J67" sqref="J67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3819,1984 +3812,1977 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="E1" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="F1" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="F1" s="32" t="s">
-        <v>150</v>
-      </c>
-      <c r="G1" s="32" t="s">
+      <c r="H1" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="I1" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="I1" s="32" t="s">
-        <v>149</v>
-      </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34" t="s">
+      <c r="F2" s="13"/>
+      <c r="G2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="34" t="s">
+      <c r="H2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="13" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34" t="s">
+      <c r="F3" s="13"/>
+      <c r="G3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="34" t="s">
+      <c r="H3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="13" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34" t="s">
+      <c r="F4" s="13"/>
+      <c r="G4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="34" t="s">
+      <c r="H4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="13" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="E5" s="34" t="s">
+      <c r="E5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34" t="s">
+      <c r="F5" s="13"/>
+      <c r="G5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="34" t="s">
+      <c r="H5" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="13" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="E6" s="34" t="s">
+      <c r="E6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34" t="s">
+      <c r="F6" s="13"/>
+      <c r="G6" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="H6" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="34" t="s">
+      <c r="H6" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="13" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="34" t="s">
+      <c r="E7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34" t="s">
+      <c r="F7" s="13"/>
+      <c r="G7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="34" t="s">
+      <c r="H7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="13" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="E8" s="34" t="s">
+      <c r="E8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34" t="s">
+      <c r="F8" s="13"/>
+      <c r="G8" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="H8" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="34" t="s">
+      <c r="H8" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="13" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D9" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="34"/>
-      <c r="G9" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="H9" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="34" t="s">
+      <c r="F9" s="13"/>
+      <c r="G9" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="13" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="34" t="s">
+      <c r="E10" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="34"/>
-      <c r="G10" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="H10" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="34" t="s">
+      <c r="F10" s="13"/>
+      <c r="G10" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D11" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="34"/>
-      <c r="G11" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="H11" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="34" t="s">
+      <c r="F11" s="13"/>
+      <c r="G11" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="34" t="s">
+      <c r="D12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34" t="s">
+      <c r="F12" s="13"/>
+      <c r="G12" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="H12" s="34" t="s">
+      <c r="H12" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="34" t="s">
+      <c r="I12" s="13" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="D13" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="34" t="s">
+      <c r="D13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34" t="s">
+      <c r="F13" s="13"/>
+      <c r="G13" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="H13" s="34" t="s">
+      <c r="H13" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="34" t="s">
+      <c r="I13" s="13" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="D14" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="34" t="s">
+      <c r="E14" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="34"/>
-      <c r="G14" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="H14" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" s="34" t="s">
+      <c r="F14" s="13"/>
+      <c r="G14" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="13" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="H15" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I15" s="34" t="s">
+      <c r="F15" s="13"/>
+      <c r="G15" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="13" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="34" t="s">
+      <c r="E16" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="34"/>
-      <c r="G16" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="H16" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" s="34" t="s">
+      <c r="F16" s="13"/>
+      <c r="G16" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="13" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="D17" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="34" t="s">
+      <c r="E17" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34" t="s">
+      <c r="F17" s="13"/>
+      <c r="G17" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="H17" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I17" s="34" t="s">
+      <c r="H17" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="13" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D18" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="34" t="s">
+      <c r="E18" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34" t="s">
+      <c r="F18" s="13"/>
+      <c r="G18" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="34" t="s">
+      <c r="H18" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="13" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="34" t="s">
+      <c r="D19" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="34"/>
-      <c r="G19" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="H19" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I19" s="34" t="s">
+      <c r="F19" s="13"/>
+      <c r="G19" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="13" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="D20" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="34" t="s">
+      <c r="D20" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34" t="s">
+      <c r="F20" s="13"/>
+      <c r="G20" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="H20" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" s="34" t="s">
+      <c r="H20" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="13" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="C21" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D21" s="34" t="s">
+      <c r="D21" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="E21" s="34" t="s">
+      <c r="E21" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34" t="s">
+      <c r="F21" s="13"/>
+      <c r="G21" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="H21" s="34" t="s">
+      <c r="H21" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="I21" s="34" t="s">
+      <c r="I21" s="13" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="E22" s="34" t="s">
+      <c r="E22" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34" t="s">
+      <c r="F22" s="13"/>
+      <c r="G22" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H22" s="34" t="s">
+      <c r="H22" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="I22" s="34" t="s">
+      <c r="I22" s="13" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C23" s="34" t="s">
+      <c r="C23" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D23" s="34" t="s">
+      <c r="D23" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="E23" s="34" t="s">
+      <c r="E23" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34" t="s">
+      <c r="F23" s="13"/>
+      <c r="G23" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="H23" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I23" s="34" t="s">
+      <c r="H23" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="13" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C24" s="34" t="s">
+      <c r="C24" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D24" s="34" t="s">
+      <c r="D24" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="34" t="s">
+      <c r="E24" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="H24" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I24" s="34" t="s">
+      <c r="F24" s="13"/>
+      <c r="G24" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="13" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="33" t="s">
+      <c r="A25" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B25" s="34" t="s">
+      <c r="B25" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="C25" s="34" t="s">
+      <c r="C25" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D25" s="34" t="s">
+      <c r="D25" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="34" t="s">
+      <c r="E25" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="H25" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I25" s="34" t="s">
+      <c r="F25" s="13"/>
+      <c r="G25" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" s="13" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="33" t="s">
+      <c r="A26" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="C26" s="34" t="s">
+      <c r="C26" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D26" s="34" t="s">
+      <c r="D26" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="34" t="s">
+      <c r="E26" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="H26" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I26" s="34" t="s">
+      <c r="F26" s="13"/>
+      <c r="G26" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" s="13" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D27" s="34" t="s">
+      <c r="D27" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E27" s="34" t="s">
+      <c r="E27" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="H27" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" s="34" t="s">
+      <c r="F27" s="13"/>
+      <c r="G27" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" s="13" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="33" t="s">
+      <c r="A28" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B28" s="34" t="s">
+      <c r="B28" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C28" s="34" t="s">
+      <c r="C28" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D28" s="34" t="s">
+      <c r="D28" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E28" s="34" t="s">
+      <c r="E28" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="H28" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I28" s="34" t="s">
+      <c r="F28" s="13"/>
+      <c r="G28" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28" s="13" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="33" t="s">
+      <c r="A29" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="C29" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="D29" s="34" t="s">
+      <c r="D29" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E29" s="34" t="s">
+      <c r="E29" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="H29" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" s="34" t="s">
+      <c r="F29" s="13"/>
+      <c r="G29" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B30" s="34" t="s">
+      <c r="B30" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C30" s="34" t="s">
+      <c r="C30" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="D30" s="34" t="s">
+      <c r="D30" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E30" s="34" t="s">
+      <c r="E30" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="H30" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I30" s="34" t="s">
+      <c r="F30" s="13"/>
+      <c r="G30" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B31" s="34" t="s">
+      <c r="B31" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="C31" s="34" t="s">
+      <c r="C31" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="D31" s="34" t="s">
+      <c r="D31" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F31" s="34"/>
-      <c r="G31" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="H31" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I31" s="34" t="s">
+      <c r="F31" s="13"/>
+      <c r="G31" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" s="13" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B32" s="34" t="s">
+      <c r="B32" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D32" s="34" t="s">
+      <c r="D32" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="E32" s="34" t="s">
+      <c r="E32" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F32" s="34"/>
-      <c r="G32" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="H32" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I32" s="34" t="s">
+      <c r="F32" s="13"/>
+      <c r="G32" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32" s="13" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B33" s="34" t="s">
+      <c r="B33" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="C33" s="34" t="s">
+      <c r="C33" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D33" s="34" t="s">
+      <c r="D33" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="E33" s="34" t="s">
+      <c r="E33" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F33" s="34"/>
-      <c r="G33" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="H33" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I33" s="34" t="s">
+      <c r="F33" s="13"/>
+      <c r="G33" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" s="13" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="33" t="s">
+      <c r="A34" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B34" s="34" t="s">
+      <c r="B34" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="C34" s="34" t="s">
+      <c r="C34" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="D34" s="34" t="s">
+      <c r="D34" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="E34" s="34" t="s">
+      <c r="E34" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F34" s="34"/>
-      <c r="G34" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="H34" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I34" s="34" t="s">
+      <c r="F34" s="13"/>
+      <c r="G34" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I34" s="13" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="33" t="s">
+      <c r="A35" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B35" s="34" t="s">
+      <c r="B35" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C35" s="34" t="s">
+      <c r="C35" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D35" s="34" t="s">
+      <c r="D35" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="E35" s="34" t="s">
+      <c r="E35" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F35" s="34"/>
-      <c r="G35" s="34" t="s">
+      <c r="F35" s="13"/>
+      <c r="G35" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="H35" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="I35" s="34" t="s">
+      <c r="H35" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I35" s="13" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="33" t="s">
+      <c r="A36" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B36" s="34" t="s">
+      <c r="B36" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C36" s="34" t="s">
+      <c r="C36" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D36" s="34" t="s">
+      <c r="D36" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="E36" s="34" t="s">
+      <c r="E36" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F36" s="35"/>
-      <c r="G36" s="35" t="s">
+      <c r="F36" s="14"/>
+      <c r="G36" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H36" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I36" s="34" t="s">
+      <c r="H36" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I36" s="13" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="32" t="s">
+      <c r="A37" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B37" s="34" t="s">
+      <c r="B37" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C37" s="34" t="s">
+      <c r="C37" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D37" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="E37" s="34" t="s">
+      <c r="D37" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F37" s="35"/>
-      <c r="G37" s="35" t="s">
+      <c r="F37" s="14"/>
+      <c r="G37" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="H37" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I37" s="34" t="s">
+      <c r="H37" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37" s="13" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="32" t="s">
+      <c r="A38" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B38" s="35" t="s">
+      <c r="B38" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="C38" s="35" t="s">
+      <c r="C38" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="D38" s="35" t="s">
+      <c r="D38" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E38" s="35" t="s">
+      <c r="E38" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F38" s="35"/>
-      <c r="G38" s="35" t="s">
+      <c r="F38" s="14"/>
+      <c r="G38" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="H38" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I38" s="34" t="s">
+      <c r="H38" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I38" s="13" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="32" t="s">
+      <c r="A39" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B39" s="35" t="s">
+      <c r="B39" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="C39" s="35" t="s">
+      <c r="C39" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="D39" s="35" t="s">
+      <c r="D39" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E39" s="35" t="s">
+      <c r="E39" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F39" s="35"/>
-      <c r="G39" s="35" t="s">
+      <c r="F39" s="14"/>
+      <c r="G39" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="H39" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I39" s="34" t="s">
+      <c r="H39" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" s="13" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="32" t="s">
+      <c r="A40" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B40" s="35" t="s">
+      <c r="B40" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="C40" s="35" t="s">
+      <c r="C40" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="D40" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E40" s="35" t="s">
+      <c r="D40" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F40" s="35"/>
-      <c r="G40" s="35" t="s">
+      <c r="F40" s="14"/>
+      <c r="G40" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="H40" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I40" s="35" t="s">
+      <c r="H40" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40" s="14" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="32" t="s">
+      <c r="A41" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B41" s="35" t="s">
+      <c r="B41" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="35" t="s">
+      <c r="C41" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="D41" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E41" s="35" t="s">
+      <c r="D41" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F41" s="35"/>
-      <c r="G41" s="35" t="s">
+      <c r="F41" s="14"/>
+      <c r="G41" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="H41" s="35" t="s">
+      <c r="H41" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="I41" s="35" t="s">
+      <c r="I41" s="14" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B42" s="35" t="s">
+      <c r="B42" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="C42" s="35" t="s">
+      <c r="C42" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="D42" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E42" s="35" t="s">
+      <c r="D42" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E42" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F42" s="35"/>
-      <c r="G42" s="35" t="s">
+      <c r="F42" s="14"/>
+      <c r="G42" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="H42" s="35" t="s">
+      <c r="H42" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="I42" s="35" t="s">
+      <c r="I42" s="14" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="32" t="s">
+      <c r="A43" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B43" s="35" t="s">
+      <c r="B43" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="C43" s="35" t="s">
+      <c r="C43" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="D43" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E43" s="35" t="s">
+      <c r="D43" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E43" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F43" s="35"/>
-      <c r="G43" s="35" t="s">
+      <c r="F43" s="14"/>
+      <c r="G43" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="H43" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I43" s="35" t="s">
+      <c r="H43" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I43" s="14" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="32" t="s">
+      <c r="A44" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B44" s="35" t="s">
+      <c r="B44" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="C44" s="35" t="s">
+      <c r="C44" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="D44" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E44" s="35" t="s">
+      <c r="D44" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E44" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F44" s="35"/>
-      <c r="G44" s="35" t="s">
+      <c r="F44" s="14"/>
+      <c r="G44" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="H44" s="35" t="s">
+      <c r="H44" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="I44" s="35" t="s">
+      <c r="I44" s="14" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="32" t="s">
+      <c r="A45" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B45" s="35" t="s">
+      <c r="B45" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="C45" s="35" t="s">
+      <c r="C45" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="D45" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E45" s="35" t="s">
+      <c r="D45" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E45" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F45" s="35"/>
-      <c r="G45" s="35" t="s">
+      <c r="F45" s="14"/>
+      <c r="G45" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="H45" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I45" s="35" t="s">
+      <c r="H45" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I45" s="14" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="32" t="s">
+      <c r="A46" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B46" s="35" t="s">
+      <c r="B46" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="C46" s="35" t="s">
+      <c r="C46" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="D46" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E46" s="35" t="s">
+      <c r="D46" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E46" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F46" s="35"/>
-      <c r="G46" s="35" t="s">
+      <c r="F46" s="14"/>
+      <c r="G46" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="H46" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I46" s="35" t="s">
+      <c r="H46" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I46" s="14" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="32" t="s">
+      <c r="A47" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B47" s="35" t="s">
+      <c r="B47" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="C47" s="35" t="s">
+      <c r="C47" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="D47" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E47" s="35" t="s">
+      <c r="D47" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E47" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F47" s="35"/>
-      <c r="G47" s="35" t="s">
+      <c r="F47" s="14"/>
+      <c r="G47" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="H47" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I47" s="35" t="s">
+      <c r="H47" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I47" s="14" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="32" t="s">
+      <c r="A48" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B48" s="35" t="s">
+      <c r="B48" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="C48" s="35" t="s">
+      <c r="C48" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="D48" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E48" s="35" t="s">
+      <c r="D48" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E48" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F48" s="35"/>
-      <c r="G48" s="35" t="s">
+      <c r="F48" s="14"/>
+      <c r="G48" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="H48" s="35" t="s">
+      <c r="H48" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="I48" s="35" t="s">
+      <c r="I48" s="14" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="32" t="s">
+      <c r="A49" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B49" s="35" t="s">
+      <c r="B49" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="C49" s="35" t="s">
+      <c r="C49" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="D49" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E49" s="35" t="s">
+      <c r="D49" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F49" s="35"/>
-      <c r="G49" s="35" t="s">
+      <c r="F49" s="14"/>
+      <c r="G49" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="H49" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I49" s="34" t="s">
+      <c r="H49" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I49" s="13" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="32" t="s">
+      <c r="A50" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B50" s="35" t="s">
+      <c r="B50" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="C50" s="35" t="s">
+      <c r="C50" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="D50" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E50" s="35" t="s">
+      <c r="D50" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F50" s="35" t="s">
+      <c r="F50" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G50" s="35" t="s">
+      <c r="G50" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="H50" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I50" s="34" t="s">
+      <c r="H50" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I50" s="13" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="32" t="s">
+      <c r="A51" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B51" s="35" t="s">
+      <c r="B51" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="C51" s="35" t="s">
+      <c r="C51" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="D51" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E51" s="35" t="s">
+      <c r="D51" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F51" s="35" t="s">
+      <c r="F51" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="G51" s="35" t="s">
+      <c r="G51" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="H51" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I51" s="34" t="s">
+      <c r="H51" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I51" s="13" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="32" t="s">
+      <c r="A52" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B52" s="35" t="s">
+      <c r="B52" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="C52" s="35" t="s">
+      <c r="C52" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="D52" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E52" s="35" t="s">
+      <c r="D52" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F52" s="35" t="s">
+      <c r="F52" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="G52" s="35" t="s">
+      <c r="G52" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="H52" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I52" s="34" t="s">
+      <c r="H52" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I52" s="13" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="32" t="s">
+      <c r="A53" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B53" s="35" t="s">
+      <c r="B53" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="C53" s="35" t="s">
+      <c r="C53" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="D53" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E53" s="35" t="s">
+      <c r="D53" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E53" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F53" s="35"/>
-      <c r="G53" s="35" t="s">
+      <c r="F53" s="14"/>
+      <c r="G53" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="H53" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I53" s="34" t="s">
+      <c r="H53" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I53" s="13" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="32" t="s">
+      <c r="A54" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B54" s="35" t="s">
+      <c r="B54" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="C54" s="35" t="s">
+      <c r="C54" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="D54" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E54" s="35" t="s">
+      <c r="D54" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E54" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F54" s="35" t="s">
+      <c r="F54" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G54" s="35" t="s">
+      <c r="G54" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="H54" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I54" s="34" t="s">
+      <c r="H54" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I54" s="13" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="32" t="s">
+      <c r="A55" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B55" s="35" t="s">
+      <c r="B55" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="C55" s="35" t="s">
+      <c r="C55" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="D55" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E55" s="35" t="s">
+      <c r="D55" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E55" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F55" s="35" t="s">
+      <c r="F55" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="G55" s="35" t="s">
+      <c r="G55" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="H55" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I55" s="34" t="s">
+      <c r="H55" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I55" s="13" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="32" t="s">
+      <c r="A56" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B56" s="35" t="s">
+      <c r="B56" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="C56" s="35" t="s">
+      <c r="C56" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="D56" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E56" s="35" t="s">
+      <c r="D56" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E56" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F56" s="35" t="s">
+      <c r="F56" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="G56" s="35" t="s">
+      <c r="G56" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="H56" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I56" s="34" t="s">
+      <c r="H56" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I56" s="13" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="32" t="s">
+      <c r="A57" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B57" s="35" t="s">
+      <c r="B57" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="C57" s="35" t="s">
+      <c r="C57" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="D57" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E57" s="35" t="s">
+      <c r="D57" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E57" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F57" s="35"/>
-      <c r="G57" s="35" t="s">
+      <c r="F57" s="14"/>
+      <c r="G57" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="H57" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I57" s="34" t="s">
+      <c r="H57" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I57" s="13" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A58" s="32" t="s">
+      <c r="A58" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B58" s="35" t="s">
+      <c r="B58" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="C58" s="35" t="s">
+      <c r="C58" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="D58" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E58" s="35" t="s">
+      <c r="D58" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E58" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F58" s="35" t="s">
+      <c r="F58" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G58" s="35" t="s">
+      <c r="G58" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="H58" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I58" s="34" t="s">
+      <c r="H58" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I58" s="13" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="32" t="s">
+      <c r="A59" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B59" s="35" t="s">
+      <c r="B59" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="C59" s="35" t="s">
+      <c r="C59" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="D59" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E59" s="35" t="s">
+      <c r="D59" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E59" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F59" s="35" t="s">
+      <c r="F59" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="G59" s="35" t="s">
+      <c r="G59" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="H59" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I59" s="34" t="s">
+      <c r="H59" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I59" s="13" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="32" t="s">
+      <c r="A60" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B60" s="35" t="s">
+      <c r="B60" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="C60" s="35" t="s">
+      <c r="C60" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="D60" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E60" s="35" t="s">
+      <c r="D60" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E60" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F60" s="35" t="s">
+      <c r="F60" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="G60" s="35" t="s">
+      <c r="G60" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="H60" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I60" s="34" t="s">
+      <c r="H60" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I60" s="13" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" s="32" t="s">
+      <c r="A61" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B61" s="35" t="s">
+      <c r="B61" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="C61" s="35" t="s">
+      <c r="C61" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="D61" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E61" s="35" t="s">
+      <c r="D61" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E61" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F61" s="35"/>
-      <c r="G61" s="35" t="s">
+      <c r="F61" s="14"/>
+      <c r="G61" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="H61" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I61" s="34" t="s">
+      <c r="H61" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I61" s="13" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" s="32" t="s">
+      <c r="A62" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B62" s="35" t="s">
+      <c r="B62" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="C62" s="35" t="s">
+      <c r="C62" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="D62" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E62" s="35" t="s">
+      <c r="D62" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E62" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F62" s="35" t="s">
+      <c r="F62" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G62" s="35" t="s">
+      <c r="G62" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="H62" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I62" s="34" t="s">
+      <c r="H62" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I62" s="13" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A63" s="32" t="s">
+      <c r="A63" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B63" s="35" t="s">
+      <c r="B63" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="C63" s="35" t="s">
+      <c r="C63" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="D63" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E63" s="35" t="s">
+      <c r="D63" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E63" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F63" s="35" t="s">
+      <c r="F63" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="G63" s="35" t="s">
+      <c r="G63" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="H63" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I63" s="34" t="s">
+      <c r="H63" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I63" s="13" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A64" s="32" t="s">
+      <c r="A64" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B64" s="35" t="s">
+      <c r="B64" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="C64" s="35" t="s">
+      <c r="C64" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="D64" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E64" s="35" t="s">
+      <c r="D64" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E64" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F64" s="35" t="s">
+      <c r="F64" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="G64" s="35" t="s">
+      <c r="G64" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="H64" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I64" s="34" t="s">
+      <c r="H64" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I64" s="13" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" s="32" t="s">
+      <c r="A65" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B65" s="35" t="s">
+      <c r="B65" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="C65" s="35" t="s">
+      <c r="C65" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="D65" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E65" s="35" t="s">
+      <c r="D65" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E65" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F65" s="35"/>
-      <c r="G65" s="35" t="s">
+      <c r="F65" s="14"/>
+      <c r="G65" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="H65" s="35" t="s">
+      <c r="H65" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="I65" s="34" t="s">
+      <c r="I65" s="13" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="32" t="s">
+      <c r="A66" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B66" s="35" t="s">
+      <c r="B66" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="C66" s="35" t="s">
+      <c r="C66" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="D66" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E66" s="35" t="s">
+      <c r="D66" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E66" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F66" s="35"/>
-      <c r="G66" s="35" t="s">
+      <c r="F66" s="14"/>
+      <c r="G66" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="H66" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I66" s="34" t="s">
+      <c r="H66" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I66" s="13" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="32" t="s">
+      <c r="A67" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B67" s="35" t="s">
+      <c r="B67" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="C67" s="35" t="s">
+      <c r="C67" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="D67" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E67" s="35" t="s">
+      <c r="D67" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E67" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F67" s="35"/>
-      <c r="G67" s="35" t="s">
-        <v>143</v>
-      </c>
-      <c r="H67" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I67" s="34" t="s">
+      <c r="F67" s="14"/>
+      <c r="G67" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="H67" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I67" s="13" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="32" t="s">
+      <c r="A68" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B68" s="35" t="s">
+      <c r="B68" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="C68" s="35" t="s">
+      <c r="C68" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="D68" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E68" s="35" t="s">
+      <c r="D68" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E68" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="F68" s="35"/>
-      <c r="G68" s="35" t="s">
+      <c r="F68" s="14"/>
+      <c r="G68" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="H68" s="35" t="s">
+      <c r="H68" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="I68" s="34" t="s">
+      <c r="I68" s="13" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A69" s="32" t="s">
+      <c r="A69" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B69" s="35" t="s">
+      <c r="B69" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="C69" s="35" t="s">
+      <c r="C69" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="D69" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E69" s="35" t="s">
+      <c r="D69" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E69" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="F69" s="35"/>
-      <c r="G69" s="35" t="s">
+      <c r="F69" s="14"/>
+      <c r="G69" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="H69" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I69" s="35" t="s">
+      <c r="H69" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I69" s="14" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A70" s="32" t="s">
+      <c r="A70" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B70" s="35" t="s">
+      <c r="B70" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="C70" s="35" t="s">
+      <c r="C70" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="D70" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E70" s="35" t="s">
+      <c r="D70" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E70" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="F70" s="35"/>
-      <c r="G70" s="35" t="s">
+      <c r="F70" s="14"/>
+      <c r="G70" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="H70" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="I70" s="34" t="s">
+      <c r="H70" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I70" s="13" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="32" t="s">
+      <c r="A71" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B71" s="35" t="s">
+      <c r="B71" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="C71" s="35" t="s">
+      <c r="C71" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="D71" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E71" s="35" t="s">
+      <c r="D71" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E71" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F71" s="35"/>
-      <c r="G71" s="35" t="s">
+      <c r="F71" s="14"/>
+      <c r="G71" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="H71" s="35" t="s">
+      <c r="H71" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="I71" s="34" t="s">
+      <c r="I71" s="13" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A72" s="32" t="s">
+      <c r="A72" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B72" s="35" t="s">
+      <c r="B72" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="C72" s="35" t="s">
+      <c r="C72" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="D72" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E72" s="35" t="s">
+      <c r="D72" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E72" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F72" s="35"/>
-      <c r="G72" s="35" t="s">
+      <c r="F72" s="14"/>
+      <c r="G72" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="H72" s="35" t="s">
-        <v>142</v>
-      </c>
-      <c r="I72" s="34" t="s">
+      <c r="H72" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I72" s="13" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B73" s="31"/>
-      <c r="C73" s="30"/>
-      <c r="D73" s="31"/>
-      <c r="E73" s="31"/>
-      <c r="F73" s="31"/>
-      <c r="G73" s="31"/>
-      <c r="H73" s="31"/>
-      <c r="I73" s="31"/>
+      <c r="C73" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>

</xml_diff>

<commit_message>
Add notebook for second experiment
</commit_message>
<xml_diff>
--- a/static/mock/titanium sols.xlsx
+++ b/static/mock/titanium sols.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexglushko/ProgProjects/ChemML/static/mock/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FBE95B1-81A4-BD43-93AA-19347C8071ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC02E81-6B58-3947-84B7-A40AF941092A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{DA8300D2-1843-2443-8DD6-A95A819FF1FD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{DA8300D2-1843-2443-8DD6-A95A819FF1FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1179,7 +1179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1226,27 +1226,6 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1277,23 +1256,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1317,7 +1308,7 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1337,7 +1328,7 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1357,7 +1348,7 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1377,7 +1368,7 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1397,7 +1388,7 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1417,7 +1408,7 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1437,7 +1428,7 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1457,7 +1448,7 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1477,10 +1468,8 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1499,7 +1488,11 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1718,18 +1711,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1E371E53-33CA-5E40-8040-CB9EEA4707B2}" name="Table2" displayName="Table2" ref="A1:I77" totalsRowShown="0" headerRowDxfId="9" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1E371E53-33CA-5E40-8040-CB9EEA4707B2}" name="Table2" displayName="Table2" ref="A1:I77" totalsRowShown="0" headerRowDxfId="10" dataDxfId="0">
   <autoFilter ref="A1:I77" xr:uid="{1E371E53-33CA-5E40-8040-CB9EEA4707B2}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{3FA7475C-433E-6D4F-B57A-00C1A515C892}" name="Composition mixtures" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{0F31B1B3-D1B1-EC4C-878B-D3AEADD20086}" name="t, °С" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{F3ADAC69-E7B8-474D-9047-06DDE55033C0}" name="t, min" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{981058E4-041A-3443-B21D-0F308E0A9A65}" name="с(acid), mol/l" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{EDCF82FF-93B9-8F4E-9258-5FC84BEFCAD0}" name="с(Ti4+), mol/l" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{43124716-5761-FA4D-B524-75FDAE619C96}" name="ultrasound " dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{C2FD9190-F3B5-6648-9534-696937C89906}" name="d, nm" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{805965AA-F35C-A949-966E-68FDEE7D2000}" name="Contents, %" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{9E1B3A05-9B84-2B4D-8FEE-A7940178837F}" name="Stability of sols, days" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{3FA7475C-433E-6D4F-B57A-00C1A515C892}" name="Composition mixtures" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{0F31B1B3-D1B1-EC4C-878B-D3AEADD20086}" name="t, °С" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{F3ADAC69-E7B8-474D-9047-06DDE55033C0}" name="t, min" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{981058E4-041A-3443-B21D-0F308E0A9A65}" name="с(acid), mol/l" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{EDCF82FF-93B9-8F4E-9258-5FC84BEFCAD0}" name="с(Ti4+), mol/l" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{43124716-5761-FA4D-B524-75FDAE619C96}" name="ultrasound " dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{C2FD9190-F3B5-6648-9534-696937C89906}" name="d, nm" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{805965AA-F35C-A949-966E-68FDEE7D2000}" name="Contents, %" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{9E1B3A05-9B84-2B4D-8FEE-A7940178837F}" name="Stability of sols, days" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2041,67 +2034,67 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="29" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="30"/>
-      <c r="I1" s="23" t="s">
+      <c r="H1" s="23"/>
+      <c r="I1" s="16" t="s">
         <v>3</v>
       </c>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="19" t="s">
+      <c r="A2" s="17"/>
+      <c r="B2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="28" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="17"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="34"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="29"/>
       <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
       <c r="G3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="25"/>
+      <c r="I3" s="18"/>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="26" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="3">
@@ -2131,7 +2124,7 @@
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
+      <c r="A5" s="31"/>
       <c r="B5" s="3">
         <v>80</v>
       </c>
@@ -2159,7 +2152,7 @@
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="3">
         <v>45</v>
       </c>
@@ -2187,7 +2180,7 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="3">
         <v>45</v>
       </c>
@@ -2215,7 +2208,7 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="26" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="3">
@@ -2245,7 +2238,7 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="3">
         <v>50</v>
       </c>
@@ -2273,7 +2266,7 @@
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="3">
         <v>80</v>
       </c>
@@ -2301,7 +2294,7 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
+      <c r="A11" s="31"/>
       <c r="B11" s="3">
         <v>45</v>
       </c>
@@ -2329,7 +2322,7 @@
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
+      <c r="A12" s="31"/>
       <c r="B12" s="3">
         <v>60</v>
       </c>
@@ -2357,7 +2350,7 @@
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
+      <c r="A13" s="31"/>
       <c r="B13" s="3">
         <v>60</v>
       </c>
@@ -2385,20 +2378,20 @@
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="20"/>
-      <c r="B14" s="19">
+      <c r="A14" s="31"/>
+      <c r="B14" s="26">
         <v>45</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="26">
         <v>130</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="F14" s="26" t="s">
         <v>14</v>
       </c>
       <c r="G14" s="6">
@@ -2407,29 +2400,29 @@
       <c r="H14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="19">
+      <c r="I14" s="26">
         <v>9</v>
       </c>
-      <c r="J14" s="22"/>
+      <c r="J14" s="30"/>
     </row>
     <row r="15" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
       <c r="G15" s="5">
         <v>45006</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="21"/>
-      <c r="J15" s="22"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="30"/>
     </row>
     <row r="16" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="3">
         <v>45</v>
       </c>
@@ -2457,7 +2450,7 @@
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
+      <c r="A17" s="31"/>
       <c r="B17" s="3">
         <v>25</v>
       </c>
@@ -2485,7 +2478,7 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
+      <c r="A18" s="31"/>
       <c r="B18" s="3">
         <v>45</v>
       </c>
@@ -2513,7 +2506,7 @@
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="3">
         <v>25</v>
       </c>
@@ -2541,7 +2534,7 @@
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
+      <c r="A20" s="31"/>
       <c r="B20" s="3">
         <v>20</v>
       </c>
@@ -2569,7 +2562,7 @@
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
+      <c r="A21" s="31"/>
       <c r="B21" s="3">
         <v>80</v>
       </c>
@@ -2597,7 +2590,7 @@
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="3">
         <v>45</v>
       </c>
@@ -2625,22 +2618,22 @@
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="19">
+      <c r="B23" s="26">
         <v>50</v>
       </c>
-      <c r="C23" s="19">
+      <c r="C23" s="26">
         <v>30</v>
       </c>
-      <c r="D23" s="19">
+      <c r="D23" s="26">
         <v>4</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="19" t="s">
+      <c r="F23" s="26" t="s">
         <v>14</v>
       </c>
       <c r="G23" s="2">
@@ -2649,29 +2642,29 @@
       <c r="H23" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I23" s="19">
+      <c r="I23" s="26">
         <v>17</v>
       </c>
-      <c r="J23" s="22"/>
+      <c r="J23" s="30"/>
     </row>
     <row r="24" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
       <c r="G24" s="3" t="s">
         <v>35</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I24" s="21"/>
-      <c r="J24" s="22"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="30"/>
     </row>
     <row r="25" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
+      <c r="A25" s="31"/>
       <c r="B25" s="3">
         <v>80</v>
       </c>
@@ -2699,7 +2692,7 @@
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
+      <c r="A26" s="31"/>
       <c r="B26" s="3">
         <v>45</v>
       </c>
@@ -2727,7 +2720,7 @@
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
+      <c r="A27" s="31"/>
       <c r="B27" s="3">
         <v>60</v>
       </c>
@@ -2755,7 +2748,7 @@
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
+      <c r="A28" s="31"/>
       <c r="B28" s="3">
         <v>60</v>
       </c>
@@ -2783,7 +2776,7 @@
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
+      <c r="A29" s="31"/>
       <c r="B29" s="3">
         <v>60</v>
       </c>
@@ -2811,7 +2804,7 @@
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
+      <c r="A30" s="31"/>
       <c r="B30" s="3">
         <v>80</v>
       </c>
@@ -2839,7 +2832,7 @@
       <c r="J30" s="1"/>
     </row>
     <row r="31" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
+      <c r="A31" s="31"/>
       <c r="B31" s="3">
         <v>60</v>
       </c>
@@ -2867,7 +2860,7 @@
       <c r="J31" s="1"/>
     </row>
     <row r="32" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="20"/>
+      <c r="A32" s="31"/>
       <c r="B32" s="3">
         <v>45</v>
       </c>
@@ -2895,7 +2888,7 @@
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
+      <c r="A33" s="31"/>
       <c r="B33" s="3">
         <v>20</v>
       </c>
@@ -2923,7 +2916,7 @@
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
+      <c r="A34" s="31"/>
       <c r="B34" s="3">
         <v>20</v>
       </c>
@@ -2951,7 +2944,7 @@
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
+      <c r="A35" s="31"/>
       <c r="B35" s="3">
         <v>20</v>
       </c>
@@ -2979,7 +2972,7 @@
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
+      <c r="A36" s="31"/>
       <c r="B36" s="3">
         <v>25</v>
       </c>
@@ -3007,7 +3000,7 @@
       <c r="J36" s="1"/>
     </row>
     <row r="37" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
+      <c r="A37" s="31"/>
       <c r="B37" s="3">
         <v>45</v>
       </c>
@@ -3035,7 +3028,7 @@
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="21"/>
+      <c r="A38" s="27"/>
       <c r="B38" s="3">
         <v>45</v>
       </c>
@@ -3063,7 +3056,7 @@
       <c r="J38" s="1"/>
     </row>
     <row r="39" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
+      <c r="A39" s="26" t="s">
         <v>43</v>
       </c>
       <c r="B39" s="3">
@@ -3093,7 +3086,7 @@
       <c r="J39" s="1"/>
     </row>
     <row r="40" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="20"/>
+      <c r="A40" s="31"/>
       <c r="B40" s="8">
         <v>80</v>
       </c>
@@ -3121,7 +3114,7 @@
       <c r="J40" s="1"/>
     </row>
     <row r="41" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="20"/>
+      <c r="A41" s="31"/>
       <c r="B41" s="8">
         <v>80</v>
       </c>
@@ -3149,7 +3142,7 @@
       <c r="J41" s="1"/>
     </row>
     <row r="42" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="20"/>
+      <c r="A42" s="31"/>
       <c r="B42" s="8">
         <v>80</v>
       </c>
@@ -3177,7 +3170,7 @@
       <c r="J42" s="1"/>
     </row>
     <row r="43" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="20"/>
+      <c r="A43" s="31"/>
       <c r="B43" s="8">
         <v>80</v>
       </c>
@@ -3205,7 +3198,7 @@
       <c r="J43" s="1"/>
     </row>
     <row r="44" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="20"/>
+      <c r="A44" s="31"/>
       <c r="B44" s="8">
         <v>85</v>
       </c>
@@ -3233,7 +3226,7 @@
       <c r="J44" s="1"/>
     </row>
     <row r="45" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="20"/>
+      <c r="A45" s="31"/>
       <c r="B45" s="8">
         <v>88</v>
       </c>
@@ -3261,7 +3254,7 @@
       <c r="J45" s="1"/>
     </row>
     <row r="46" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="20"/>
+      <c r="A46" s="31"/>
       <c r="B46" s="8">
         <v>88</v>
       </c>
@@ -3289,7 +3282,7 @@
       <c r="J46" s="1"/>
     </row>
     <row r="47" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="20"/>
+      <c r="A47" s="31"/>
       <c r="B47" s="8">
         <v>89</v>
       </c>
@@ -3317,7 +3310,7 @@
       <c r="J47" s="1"/>
     </row>
     <row r="48" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="20"/>
+      <c r="A48" s="31"/>
       <c r="B48" s="8">
         <v>89</v>
       </c>
@@ -3345,7 +3338,7 @@
       <c r="J48" s="1"/>
     </row>
     <row r="49" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="20"/>
+      <c r="A49" s="31"/>
       <c r="B49" s="8">
         <v>93</v>
       </c>
@@ -3373,7 +3366,7 @@
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="20"/>
+      <c r="A50" s="31"/>
       <c r="B50" s="8">
         <v>93</v>
       </c>
@@ -3401,17 +3394,17 @@
       <c r="J50" s="1"/>
     </row>
     <row r="51" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="20"/>
-      <c r="B51" s="16">
+      <c r="A51" s="31"/>
+      <c r="B51" s="32">
         <v>71</v>
       </c>
-      <c r="C51" s="16">
+      <c r="C51" s="32">
         <v>9</v>
       </c>
-      <c r="D51" s="16" t="s">
+      <c r="D51" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="E51" s="16" t="s">
+      <c r="E51" s="32" t="s">
         <v>44</v>
       </c>
       <c r="F51" s="8" t="s">
@@ -3429,11 +3422,11 @@
       <c r="J51" s="1"/>
     </row>
     <row r="52" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="20"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="17"/>
-      <c r="D52" s="17"/>
-      <c r="E52" s="17"/>
+      <c r="A52" s="31"/>
+      <c r="B52" s="33"/>
+      <c r="C52" s="33"/>
+      <c r="D52" s="33"/>
+      <c r="E52" s="33"/>
       <c r="F52" s="8" t="s">
         <v>13</v>
       </c>
@@ -3449,11 +3442,11 @@
       <c r="J52" s="1"/>
     </row>
     <row r="53" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="20"/>
-      <c r="B53" s="17"/>
-      <c r="C53" s="17"/>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17"/>
+      <c r="A53" s="31"/>
+      <c r="B53" s="33"/>
+      <c r="C53" s="33"/>
+      <c r="D53" s="33"/>
+      <c r="E53" s="33"/>
       <c r="F53" s="8">
         <v>1</v>
       </c>
@@ -3469,11 +3462,11 @@
       <c r="J53" s="1"/>
     </row>
     <row r="54" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="20"/>
-      <c r="B54" s="18"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="18"/>
+      <c r="A54" s="31"/>
+      <c r="B54" s="34"/>
+      <c r="C54" s="34"/>
+      <c r="D54" s="34"/>
+      <c r="E54" s="34"/>
       <c r="F54" s="9">
         <v>45047</v>
       </c>
@@ -3489,17 +3482,17 @@
       <c r="J54" s="1"/>
     </row>
     <row r="55" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="20"/>
-      <c r="B55" s="16">
+      <c r="A55" s="31"/>
+      <c r="B55" s="32">
         <v>71</v>
       </c>
-      <c r="C55" s="16">
+      <c r="C55" s="32">
         <v>10</v>
       </c>
-      <c r="D55" s="16" t="s">
+      <c r="D55" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="E55" s="16" t="s">
+      <c r="E55" s="32" t="s">
         <v>44</v>
       </c>
       <c r="F55" s="8" t="s">
@@ -3517,11 +3510,11 @@
       <c r="J55" s="1"/>
     </row>
     <row r="56" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="20"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17"/>
+      <c r="A56" s="31"/>
+      <c r="B56" s="33"/>
+      <c r="C56" s="33"/>
+      <c r="D56" s="33"/>
+      <c r="E56" s="33"/>
       <c r="F56" s="8" t="s">
         <v>13</v>
       </c>
@@ -3537,11 +3530,11 @@
       <c r="J56" s="1"/>
     </row>
     <row r="57" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="20"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="17"/>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17"/>
+      <c r="A57" s="31"/>
+      <c r="B57" s="33"/>
+      <c r="C57" s="33"/>
+      <c r="D57" s="33"/>
+      <c r="E57" s="33"/>
       <c r="F57" s="8">
         <v>1</v>
       </c>
@@ -3557,11 +3550,11 @@
       <c r="J57" s="1"/>
     </row>
     <row r="58" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="20"/>
-      <c r="B58" s="18"/>
-      <c r="C58" s="18"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="18"/>
+      <c r="A58" s="31"/>
+      <c r="B58" s="34"/>
+      <c r="C58" s="34"/>
+      <c r="D58" s="34"/>
+      <c r="E58" s="34"/>
       <c r="F58" s="9">
         <v>45047</v>
       </c>
@@ -3577,17 +3570,17 @@
       <c r="J58" s="1"/>
     </row>
     <row r="59" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="20"/>
-      <c r="B59" s="16">
+      <c r="A59" s="31"/>
+      <c r="B59" s="32">
         <v>71</v>
       </c>
-      <c r="C59" s="16">
+      <c r="C59" s="32">
         <v>11</v>
       </c>
-      <c r="D59" s="16" t="s">
+      <c r="D59" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="E59" s="16" t="s">
+      <c r="E59" s="32" t="s">
         <v>44</v>
       </c>
       <c r="F59" s="8" t="s">
@@ -3605,11 +3598,11 @@
       <c r="J59" s="1"/>
     </row>
     <row r="60" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="20"/>
-      <c r="B60" s="17"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
+      <c r="A60" s="31"/>
+      <c r="B60" s="33"/>
+      <c r="C60" s="33"/>
+      <c r="D60" s="33"/>
+      <c r="E60" s="33"/>
       <c r="F60" s="8" t="s">
         <v>13</v>
       </c>
@@ -3625,11 +3618,11 @@
       <c r="J60" s="1"/>
     </row>
     <row r="61" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="20"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="17"/>
-      <c r="D61" s="17"/>
-      <c r="E61" s="17"/>
+      <c r="A61" s="31"/>
+      <c r="B61" s="33"/>
+      <c r="C61" s="33"/>
+      <c r="D61" s="33"/>
+      <c r="E61" s="33"/>
       <c r="F61" s="8">
         <v>1</v>
       </c>
@@ -3645,11 +3638,11 @@
       <c r="J61" s="1"/>
     </row>
     <row r="62" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="20"/>
-      <c r="B62" s="18"/>
-      <c r="C62" s="18"/>
-      <c r="D62" s="18"/>
-      <c r="E62" s="18"/>
+      <c r="A62" s="31"/>
+      <c r="B62" s="34"/>
+      <c r="C62" s="34"/>
+      <c r="D62" s="34"/>
+      <c r="E62" s="34"/>
       <c r="F62" s="9">
         <v>45047</v>
       </c>
@@ -3665,17 +3658,17 @@
       <c r="J62" s="1"/>
     </row>
     <row r="63" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="20"/>
-      <c r="B63" s="16">
+      <c r="A63" s="31"/>
+      <c r="B63" s="32">
         <v>71</v>
       </c>
-      <c r="C63" s="16">
+      <c r="C63" s="32">
         <v>12</v>
       </c>
-      <c r="D63" s="16" t="s">
+      <c r="D63" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="E63" s="16" t="s">
+      <c r="E63" s="32" t="s">
         <v>44</v>
       </c>
       <c r="F63" s="8" t="s">
@@ -3693,11 +3686,11 @@
       <c r="J63" s="1"/>
     </row>
     <row r="64" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="20"/>
-      <c r="B64" s="17"/>
-      <c r="C64" s="17"/>
-      <c r="D64" s="17"/>
-      <c r="E64" s="17"/>
+      <c r="A64" s="31"/>
+      <c r="B64" s="33"/>
+      <c r="C64" s="33"/>
+      <c r="D64" s="33"/>
+      <c r="E64" s="33"/>
       <c r="F64" s="8" t="s">
         <v>13</v>
       </c>
@@ -3713,11 +3706,11 @@
       <c r="J64" s="1"/>
     </row>
     <row r="65" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="20"/>
-      <c r="B65" s="17"/>
-      <c r="C65" s="17"/>
-      <c r="D65" s="17"/>
-      <c r="E65" s="17"/>
+      <c r="A65" s="31"/>
+      <c r="B65" s="33"/>
+      <c r="C65" s="33"/>
+      <c r="D65" s="33"/>
+      <c r="E65" s="33"/>
       <c r="F65" s="8">
         <v>1</v>
       </c>
@@ -3733,11 +3726,11 @@
       <c r="J65" s="1"/>
     </row>
     <row r="66" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="20"/>
-      <c r="B66" s="18"/>
-      <c r="C66" s="18"/>
-      <c r="D66" s="18"/>
-      <c r="E66" s="18"/>
+      <c r="A66" s="31"/>
+      <c r="B66" s="34"/>
+      <c r="C66" s="34"/>
+      <c r="D66" s="34"/>
+      <c r="E66" s="34"/>
       <c r="F66" s="9">
         <v>45047</v>
       </c>
@@ -3753,7 +3746,7 @@
       <c r="J66" s="1"/>
     </row>
     <row r="67" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="20"/>
+      <c r="A67" s="31"/>
       <c r="B67" s="8">
         <v>65</v>
       </c>
@@ -3781,7 +3774,7 @@
       <c r="J67" s="1"/>
     </row>
     <row r="68" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="20"/>
+      <c r="A68" s="31"/>
       <c r="B68" s="8">
         <v>75</v>
       </c>
@@ -3809,7 +3802,7 @@
       <c r="J68" s="1"/>
     </row>
     <row r="69" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="20"/>
+      <c r="A69" s="31"/>
       <c r="B69" s="8">
         <v>85</v>
       </c>
@@ -3837,7 +3830,7 @@
       <c r="J69" s="1"/>
     </row>
     <row r="70" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="20"/>
+      <c r="A70" s="31"/>
       <c r="B70" s="8">
         <v>70</v>
       </c>
@@ -3865,7 +3858,7 @@
       <c r="J70" s="1"/>
     </row>
     <row r="71" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="20"/>
+      <c r="A71" s="31"/>
       <c r="B71" s="8">
         <v>70</v>
       </c>
@@ -3893,7 +3886,7 @@
       <c r="J71" s="1"/>
     </row>
     <row r="72" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="20"/>
+      <c r="A72" s="31"/>
       <c r="B72" s="8">
         <v>70</v>
       </c>
@@ -3921,7 +3914,7 @@
       <c r="J72" s="1"/>
     </row>
     <row r="73" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="20"/>
+      <c r="A73" s="31"/>
       <c r="B73" s="8">
         <v>70</v>
       </c>
@@ -3949,7 +3942,7 @@
       <c r="J73" s="1"/>
     </row>
     <row r="74" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="21"/>
+      <c r="A74" s="27"/>
       <c r="B74" s="8">
         <v>80</v>
       </c>
@@ -3978,23 +3971,15 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="G1:H2"/>
-    <mergeCell ref="I1:I3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="A23:A38"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A22"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="D63:D66"/>
+    <mergeCell ref="E63:E66"/>
+    <mergeCell ref="E55:E58"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="C59:C62"/>
+    <mergeCell ref="D59:D62"/>
+    <mergeCell ref="E59:E62"/>
     <mergeCell ref="A39:A74"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:E15"/>
@@ -4011,15 +3996,23 @@
     <mergeCell ref="B55:B58"/>
     <mergeCell ref="C55:C58"/>
     <mergeCell ref="D55:D58"/>
-    <mergeCell ref="B63:B66"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="D63:D66"/>
-    <mergeCell ref="E63:E66"/>
-    <mergeCell ref="E55:E58"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="C59:C62"/>
-    <mergeCell ref="D59:D62"/>
-    <mergeCell ref="E59:E62"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="A23:A38"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A22"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:H2"/>
+    <mergeCell ref="I1:I3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6030,7 +6023,7 @@
   <dimension ref="A1:I77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="K82" sqref="K82"/>
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6044,2233 +6037,2233 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="H1" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="12" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="38">
+      <c r="B2" s="13">
         <v>45</v>
       </c>
-      <c r="C2" s="38">
+      <c r="C2" s="13">
         <v>60</v>
       </c>
-      <c r="D2" s="38">
+      <c r="D2" s="13">
         <v>4</v>
       </c>
-      <c r="E2" s="38">
+      <c r="E2" s="13">
         <v>0.5</v>
       </c>
-      <c r="F2" s="38">
+      <c r="F2" s="13">
         <v>0</v>
       </c>
-      <c r="G2" s="38">
+      <c r="G2" s="13">
         <v>618.5</v>
       </c>
-      <c r="H2" s="38">
+      <c r="H2" s="13">
         <v>100</v>
       </c>
-      <c r="I2" s="38">
+      <c r="I2" s="13">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="38">
+      <c r="B3" s="13">
         <v>80</v>
       </c>
-      <c r="C3" s="38">
+      <c r="C3" s="13">
         <v>10</v>
       </c>
-      <c r="D3" s="38">
+      <c r="D3" s="13">
         <v>4</v>
       </c>
-      <c r="E3" s="38">
+      <c r="E3" s="13">
         <v>0.5</v>
       </c>
-      <c r="F3" s="38">
+      <c r="F3" s="13">
         <v>0</v>
       </c>
-      <c r="G3" s="38">
+      <c r="G3" s="13">
         <v>978.1</v>
       </c>
-      <c r="H3" s="38">
+      <c r="H3" s="13">
         <v>100</v>
       </c>
-      <c r="I3" s="38">
+      <c r="I3" s="13">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="38">
+      <c r="B4" s="13">
         <v>45</v>
       </c>
-      <c r="C4" s="38">
+      <c r="C4" s="13">
         <v>20</v>
       </c>
-      <c r="D4" s="38">
+      <c r="D4" s="13">
         <v>4</v>
       </c>
-      <c r="E4" s="38">
+      <c r="E4" s="13">
         <v>0.5</v>
       </c>
-      <c r="F4" s="38">
+      <c r="F4" s="13">
         <v>0</v>
       </c>
-      <c r="G4" s="38">
+      <c r="G4" s="13">
         <v>2</v>
       </c>
-      <c r="H4" s="38">
+      <c r="H4" s="13">
         <v>100</v>
       </c>
-      <c r="I4" s="38">
+      <c r="I4" s="13">
         <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="38">
+      <c r="B5" s="13">
         <v>45</v>
       </c>
-      <c r="C5" s="38">
+      <c r="C5" s="13">
         <v>20</v>
       </c>
-      <c r="D5" s="38">
+      <c r="D5" s="13">
         <v>4</v>
       </c>
-      <c r="E5" s="38">
+      <c r="E5" s="13">
         <v>0.47</v>
       </c>
-      <c r="F5" s="38">
+      <c r="F5" s="13">
         <v>0</v>
       </c>
-      <c r="G5" s="38">
+      <c r="G5" s="13">
         <v>2.6280000000000001</v>
       </c>
-      <c r="H5" s="38">
+      <c r="H5" s="13">
         <v>100</v>
       </c>
-      <c r="I5" s="38">
+      <c r="I5" s="13">
         <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="38">
+      <c r="B6" s="13">
         <v>50</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6" s="13">
         <v>20</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6" s="13">
         <v>4</v>
       </c>
-      <c r="E6" s="38">
+      <c r="E6" s="13">
         <v>0.2</v>
       </c>
-      <c r="F6" s="38">
+      <c r="F6" s="13">
         <v>0</v>
       </c>
-      <c r="G6" s="38">
+      <c r="G6" s="13">
         <v>1712</v>
       </c>
-      <c r="H6" s="38">
+      <c r="H6" s="13">
         <v>100</v>
       </c>
-      <c r="I6" s="38">
+      <c r="I6" s="13">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="38">
+      <c r="B7" s="13">
         <v>50</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="13">
         <v>30</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="13">
         <v>4</v>
       </c>
-      <c r="E7" s="38">
+      <c r="E7" s="13">
         <v>0.2</v>
       </c>
-      <c r="F7" s="38">
+      <c r="F7" s="13">
         <v>0</v>
       </c>
-      <c r="G7" s="38">
+      <c r="G7" s="13">
         <v>889.6</v>
       </c>
-      <c r="H7" s="38">
+      <c r="H7" s="13">
         <v>100</v>
       </c>
-      <c r="I7" s="38">
+      <c r="I7" s="13">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="38">
+      <c r="B8" s="13">
         <v>80</v>
       </c>
-      <c r="C8" s="38">
+      <c r="C8" s="13">
         <v>20</v>
       </c>
-      <c r="D8" s="38">
+      <c r="D8" s="13">
         <v>4</v>
       </c>
-      <c r="E8" s="38">
+      <c r="E8" s="13">
         <v>0.2</v>
       </c>
-      <c r="F8" s="38">
+      <c r="F8" s="13">
         <v>0</v>
       </c>
-      <c r="G8" s="38">
+      <c r="G8" s="13">
         <v>1.7</v>
       </c>
-      <c r="H8" s="38">
+      <c r="H8" s="13">
         <v>100</v>
       </c>
-      <c r="I8" s="38">
+      <c r="I8" s="13">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="38">
+      <c r="B9" s="13">
         <v>45</v>
       </c>
-      <c r="C9" s="38">
+      <c r="C9" s="13">
         <v>60</v>
       </c>
-      <c r="D9" s="38">
+      <c r="D9" s="13">
         <v>0.3</v>
       </c>
-      <c r="E9" s="38">
+      <c r="E9" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F9" s="38">
+      <c r="F9" s="13">
         <v>0</v>
       </c>
-      <c r="G9" s="38">
+      <c r="G9" s="13">
         <v>2000</v>
       </c>
-      <c r="H9" s="38">
+      <c r="H9" s="13">
         <v>100</v>
       </c>
-      <c r="I9" s="38">
+      <c r="I9" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="38">
+      <c r="B10" s="13">
         <v>60</v>
       </c>
-      <c r="C10" s="38">
+      <c r="C10" s="13">
         <v>60</v>
       </c>
-      <c r="D10" s="38">
+      <c r="D10" s="13">
         <v>0.3</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F10" s="13">
         <v>0</v>
       </c>
-      <c r="G10" s="38">
+      <c r="G10" s="13">
         <v>2000</v>
       </c>
-      <c r="H10" s="38">
+      <c r="H10" s="13">
         <v>100</v>
       </c>
-      <c r="I10" s="38">
+      <c r="I10" s="13">
         <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="38">
+      <c r="B11" s="13">
         <v>60</v>
       </c>
-      <c r="C11" s="38">
+      <c r="C11" s="13">
         <v>15</v>
       </c>
-      <c r="D11" s="38">
+      <c r="D11" s="13">
         <v>0.3</v>
       </c>
-      <c r="E11" s="38">
+      <c r="E11" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F11" s="38">
+      <c r="F11" s="13">
         <v>0</v>
       </c>
-      <c r="G11" s="38">
+      <c r="G11" s="13">
         <v>2000</v>
       </c>
-      <c r="H11" s="38">
+      <c r="H11" s="13">
         <v>100</v>
       </c>
-      <c r="I11" s="38">
+      <c r="I11" s="13">
         <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="38">
+      <c r="B12" s="13">
         <v>45</v>
       </c>
-      <c r="C12" s="38">
+      <c r="C12" s="13">
         <v>130</v>
       </c>
-      <c r="D12" s="38">
+      <c r="D12" s="13">
         <v>0.1</v>
       </c>
-      <c r="E12" s="38">
+      <c r="E12" s="13">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F12" s="38">
+      <c r="F12" s="13">
         <v>0</v>
       </c>
-      <c r="G12" s="38">
+      <c r="G12" s="13">
         <v>8.3000000000000007</v>
       </c>
-      <c r="H12" s="38">
+      <c r="H12" s="13">
         <v>99.5</v>
       </c>
-      <c r="I12" s="38">
+      <c r="I12" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="38">
+      <c r="B13" s="13">
         <v>45</v>
       </c>
-      <c r="C13" s="38">
+      <c r="C13" s="13">
         <v>130</v>
       </c>
-      <c r="D13" s="38">
+      <c r="D13" s="13">
         <v>0.1</v>
       </c>
-      <c r="E13" s="38">
+      <c r="E13" s="13">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F13" s="38">
+      <c r="F13" s="13">
         <v>0</v>
       </c>
-      <c r="G13" s="38">
+      <c r="G13" s="13">
         <v>21.3</v>
       </c>
-      <c r="H13" s="38">
+      <c r="H13" s="13">
         <v>0.5</v>
       </c>
-      <c r="I13" s="38">
+      <c r="I13" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="38">
+      <c r="B14" s="13">
         <v>45</v>
       </c>
-      <c r="C14" s="38">
+      <c r="C14" s="13">
         <v>83</v>
       </c>
-      <c r="D14" s="38">
+      <c r="D14" s="13">
         <v>0.26</v>
       </c>
-      <c r="E14" s="38">
+      <c r="E14" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F14" s="38">
+      <c r="F14" s="13">
         <v>0</v>
       </c>
-      <c r="G14" s="38">
+      <c r="G14" s="13">
         <v>2000</v>
       </c>
-      <c r="H14" s="38">
+      <c r="H14" s="13">
         <v>100</v>
       </c>
-      <c r="I14" s="38">
+      <c r="I14" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="38">
+      <c r="B15" s="13">
         <v>25</v>
       </c>
-      <c r="C15" s="38">
+      <c r="C15" s="13">
         <v>61</v>
       </c>
-      <c r="D15" s="38">
+      <c r="D15" s="13">
         <v>0.26</v>
       </c>
-      <c r="E15" s="38">
+      <c r="E15" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F15" s="38">
+      <c r="F15" s="13">
         <v>0</v>
       </c>
-      <c r="G15" s="38">
+      <c r="G15" s="13">
         <v>2000</v>
       </c>
-      <c r="H15" s="38">
+      <c r="H15" s="13">
         <v>100</v>
       </c>
-      <c r="I15" s="38">
+      <c r="I15" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="38">
+      <c r="B16" s="13">
         <v>45</v>
       </c>
-      <c r="C16" s="38">
+      <c r="C16" s="13">
         <v>56</v>
       </c>
-      <c r="D16" s="38">
+      <c r="D16" s="13">
         <v>0.26</v>
       </c>
-      <c r="E16" s="38">
+      <c r="E16" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F16" s="38">
+      <c r="F16" s="13">
         <v>0</v>
       </c>
-      <c r="G16" s="38">
+      <c r="G16" s="13">
         <v>2000</v>
       </c>
-      <c r="H16" s="38">
+      <c r="H16" s="13">
         <v>100</v>
       </c>
-      <c r="I16" s="38">
+      <c r="I16" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="38">
+      <c r="B17" s="13">
         <v>25</v>
       </c>
-      <c r="C17" s="38">
+      <c r="C17" s="13">
         <v>60</v>
       </c>
-      <c r="D17" s="38">
+      <c r="D17" s="13">
         <v>0.53</v>
       </c>
-      <c r="E17" s="38">
+      <c r="E17" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F17" s="38">
+      <c r="F17" s="13">
         <v>0</v>
       </c>
-      <c r="G17" s="38">
+      <c r="G17" s="13">
         <v>832.4</v>
       </c>
-      <c r="H17" s="38">
+      <c r="H17" s="13">
         <v>100</v>
       </c>
-      <c r="I17" s="38">
+      <c r="I17" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="38">
+      <c r="B18" s="13">
         <v>20</v>
       </c>
-      <c r="C18" s="38">
+      <c r="C18" s="13">
         <v>58</v>
       </c>
-      <c r="D18" s="38">
+      <c r="D18" s="13">
         <v>0.53</v>
       </c>
-      <c r="E18" s="38">
+      <c r="E18" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F18" s="38">
+      <c r="F18" s="13">
         <v>0</v>
       </c>
-      <c r="G18" s="38">
+      <c r="G18" s="13">
         <v>716.2</v>
       </c>
-      <c r="H18" s="38">
+      <c r="H18" s="13">
         <v>100</v>
       </c>
-      <c r="I18" s="38">
+      <c r="I18" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="38">
+      <c r="B19" s="13">
         <v>80</v>
       </c>
-      <c r="C19" s="38">
+      <c r="C19" s="13">
         <v>60</v>
       </c>
-      <c r="D19" s="38">
+      <c r="D19" s="13">
         <v>0.1</v>
       </c>
-      <c r="E19" s="38">
+      <c r="E19" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F19" s="38">
+      <c r="F19" s="13">
         <v>0</v>
       </c>
-      <c r="G19" s="38">
+      <c r="G19" s="13">
         <v>2000</v>
       </c>
-      <c r="H19" s="38">
+      <c r="H19" s="13">
         <v>100</v>
       </c>
-      <c r="I19" s="38">
+      <c r="I19" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="38">
+      <c r="B20" s="13">
         <v>45</v>
       </c>
-      <c r="C20" s="38">
+      <c r="C20" s="13">
         <v>130</v>
       </c>
-      <c r="D20" s="38">
+      <c r="D20" s="13">
         <v>0.1</v>
       </c>
-      <c r="E20" s="38">
+      <c r="E20" s="13">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F20" s="38">
+      <c r="F20" s="13">
         <v>0</v>
       </c>
-      <c r="G20" s="38">
+      <c r="G20" s="13">
         <v>5.4</v>
       </c>
-      <c r="H20" s="38">
+      <c r="H20" s="13">
         <v>100</v>
       </c>
-      <c r="I20" s="38">
+      <c r="I20" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A21" s="37" t="s">
+      <c r="A21" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="38">
+      <c r="B21" s="13">
         <v>50</v>
       </c>
-      <c r="C21" s="38">
+      <c r="C21" s="13">
         <v>30</v>
       </c>
-      <c r="D21" s="38">
+      <c r="D21" s="13">
         <v>4</v>
       </c>
-      <c r="E21" s="38">
+      <c r="E21" s="13">
         <v>0.3</v>
       </c>
-      <c r="F21" s="38">
+      <c r="F21" s="13">
         <v>0</v>
       </c>
-      <c r="G21" s="38">
+      <c r="G21" s="13">
         <v>2159</v>
       </c>
-      <c r="H21" s="38">
+      <c r="H21" s="13">
         <v>41.6</v>
       </c>
-      <c r="I21" s="38">
+      <c r="I21" s="13">
         <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="38">
+      <c r="B22" s="13">
         <v>50</v>
       </c>
-      <c r="C22" s="38">
+      <c r="C22" s="13">
         <v>30</v>
       </c>
-      <c r="D22" s="38">
+      <c r="D22" s="13">
         <v>4</v>
       </c>
-      <c r="E22" s="38">
+      <c r="E22" s="13">
         <v>0.3</v>
       </c>
-      <c r="F22" s="38">
+      <c r="F22" s="13">
         <v>0</v>
       </c>
-      <c r="G22" s="38">
+      <c r="G22" s="13">
         <v>487.2</v>
       </c>
-      <c r="H22" s="38">
+      <c r="H22" s="13">
         <v>58.4</v>
       </c>
-      <c r="I22" s="38"/>
+      <c r="I22" s="13"/>
     </row>
     <row r="23" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A23" s="37" t="s">
+      <c r="A23" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="38">
+      <c r="B23" s="13">
         <v>80</v>
       </c>
-      <c r="C23" s="38">
+      <c r="C23" s="13">
         <v>20</v>
       </c>
-      <c r="D23" s="38">
+      <c r="D23" s="13">
         <v>4</v>
       </c>
-      <c r="E23" s="38">
+      <c r="E23" s="13">
         <v>0.3</v>
       </c>
-      <c r="F23" s="38">
+      <c r="F23" s="13">
         <v>0</v>
       </c>
-      <c r="G23" s="38">
+      <c r="G23" s="13">
         <v>1021</v>
       </c>
-      <c r="H23" s="38">
+      <c r="H23" s="13">
         <v>100</v>
       </c>
-      <c r="I23" s="38">
+      <c r="I23" s="13">
         <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="38">
+      <c r="B24" s="13">
         <v>45</v>
       </c>
-      <c r="C24" s="38">
+      <c r="C24" s="13">
         <v>60</v>
       </c>
-      <c r="D24" s="38">
+      <c r="D24" s="13">
         <v>0.3</v>
       </c>
-      <c r="E24" s="38">
+      <c r="E24" s="13">
         <v>0.35</v>
       </c>
-      <c r="F24" s="38">
+      <c r="F24" s="13">
         <v>0</v>
       </c>
-      <c r="G24" s="38">
+      <c r="G24" s="13">
         <v>2000</v>
       </c>
-      <c r="H24" s="38">
+      <c r="H24" s="13">
         <v>100</v>
       </c>
-      <c r="I24" s="38">
+      <c r="I24" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A25" s="37" t="s">
+      <c r="A25" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="38">
+      <c r="B25" s="13">
         <v>60</v>
       </c>
-      <c r="C25" s="38">
+      <c r="C25" s="13">
         <v>60</v>
       </c>
-      <c r="D25" s="38">
+      <c r="D25" s="13">
         <v>0.3</v>
       </c>
-      <c r="E25" s="38">
+      <c r="E25" s="13">
         <v>0.35</v>
       </c>
-      <c r="F25" s="38">
+      <c r="F25" s="13">
         <v>0</v>
       </c>
-      <c r="G25" s="38">
+      <c r="G25" s="13">
         <v>2000</v>
       </c>
-      <c r="H25" s="38">
+      <c r="H25" s="13">
         <v>100</v>
       </c>
-      <c r="I25" s="38">
+      <c r="I25" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A26" s="37" t="s">
+      <c r="A26" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="38">
+      <c r="B26" s="13">
         <v>60</v>
       </c>
-      <c r="C26" s="38">
+      <c r="C26" s="13">
         <v>30</v>
       </c>
-      <c r="D26" s="38">
+      <c r="D26" s="13">
         <v>0.3</v>
       </c>
-      <c r="E26" s="38">
+      <c r="E26" s="13">
         <v>0.35</v>
       </c>
-      <c r="F26" s="38">
+      <c r="F26" s="13">
         <v>0</v>
       </c>
-      <c r="G26" s="38">
+      <c r="G26" s="13">
         <v>2000</v>
       </c>
-      <c r="H26" s="38">
+      <c r="H26" s="13">
         <v>100</v>
       </c>
-      <c r="I26" s="38">
+      <c r="I26" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="38">
+      <c r="B27" s="13">
         <v>60</v>
       </c>
-      <c r="C27" s="38">
+      <c r="C27" s="13">
         <v>60</v>
       </c>
-      <c r="D27" s="38">
+      <c r="D27" s="13">
         <v>0.3</v>
       </c>
-      <c r="E27" s="38">
+      <c r="E27" s="13">
         <v>0.17</v>
       </c>
-      <c r="F27" s="38">
+      <c r="F27" s="13">
         <v>0</v>
       </c>
-      <c r="G27" s="38">
+      <c r="G27" s="13">
         <v>2000</v>
       </c>
-      <c r="H27" s="38">
+      <c r="H27" s="13">
         <v>100</v>
       </c>
-      <c r="I27" s="38">
+      <c r="I27" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="38">
+      <c r="B28" s="13">
         <v>80</v>
       </c>
-      <c r="C28" s="38">
+      <c r="C28" s="13">
         <v>20</v>
       </c>
-      <c r="D28" s="38">
+      <c r="D28" s="13">
         <v>0.3</v>
       </c>
-      <c r="E28" s="38">
+      <c r="E28" s="13">
         <v>0.17</v>
       </c>
-      <c r="F28" s="38">
+      <c r="F28" s="13">
         <v>0</v>
       </c>
-      <c r="G28" s="38">
+      <c r="G28" s="13">
         <v>2000</v>
       </c>
-      <c r="H28" s="38">
+      <c r="H28" s="13">
         <v>100</v>
       </c>
-      <c r="I28" s="38">
+      <c r="I28" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="38">
+      <c r="B29" s="13">
         <v>60</v>
       </c>
-      <c r="C29" s="38">
+      <c r="C29" s="13">
         <v>40</v>
       </c>
-      <c r="D29" s="38">
+      <c r="D29" s="13">
         <v>0.3</v>
       </c>
-      <c r="E29" s="38">
+      <c r="E29" s="13">
         <v>0.17</v>
       </c>
-      <c r="F29" s="38">
+      <c r="F29" s="13">
         <v>0</v>
       </c>
-      <c r="G29" s="38">
+      <c r="G29" s="13">
         <v>2000</v>
       </c>
-      <c r="H29" s="38">
+      <c r="H29" s="13">
         <v>100</v>
       </c>
-      <c r="I29" s="38">
+      <c r="I29" s="13">
         <v>0.5</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A30" s="37" t="s">
+      <c r="A30" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="38">
+      <c r="B30" s="13">
         <v>45</v>
       </c>
-      <c r="C30" s="38">
+      <c r="C30" s="13">
         <v>70</v>
       </c>
-      <c r="D30" s="38">
+      <c r="D30" s="13">
         <v>0.8</v>
       </c>
-      <c r="E30" s="38">
+      <c r="E30" s="13">
         <v>0.17</v>
       </c>
-      <c r="F30" s="38">
+      <c r="F30" s="13">
         <v>0</v>
       </c>
-      <c r="G30" s="38">
+      <c r="G30" s="13">
         <v>2000</v>
       </c>
-      <c r="H30" s="38">
+      <c r="H30" s="13">
         <v>100</v>
       </c>
-      <c r="I30" s="38">
+      <c r="I30" s="13">
         <v>0.5</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A31" s="37" t="s">
+      <c r="A31" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="38">
+      <c r="B31" s="13">
         <v>20</v>
       </c>
-      <c r="C31" s="38">
+      <c r="C31" s="13">
         <v>50</v>
       </c>
-      <c r="D31" s="38">
+      <c r="D31" s="13">
         <v>1.58</v>
       </c>
-      <c r="E31" s="38">
+      <c r="E31" s="13">
         <v>0.15</v>
       </c>
-      <c r="F31" s="38">
+      <c r="F31" s="13">
         <v>0</v>
       </c>
-      <c r="G31" s="38">
+      <c r="G31" s="13">
         <v>2000</v>
       </c>
-      <c r="H31" s="38">
+      <c r="H31" s="13">
         <v>100</v>
       </c>
-      <c r="I31" s="38">
+      <c r="I31" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="38">
+      <c r="B32" s="13">
         <v>20</v>
       </c>
-      <c r="C32" s="38">
+      <c r="C32" s="13">
         <v>80</v>
       </c>
-      <c r="D32" s="38">
+      <c r="D32" s="13">
         <v>1.58</v>
       </c>
-      <c r="E32" s="38">
+      <c r="E32" s="13">
         <v>0.15</v>
       </c>
-      <c r="F32" s="38">
+      <c r="F32" s="13">
         <v>0</v>
       </c>
-      <c r="G32" s="38">
+      <c r="G32" s="13">
         <v>2000</v>
       </c>
-      <c r="H32" s="38">
+      <c r="H32" s="13">
         <v>100</v>
       </c>
-      <c r="I32" s="38">
+      <c r="I32" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="38">
+      <c r="B33" s="13">
         <v>20</v>
       </c>
-      <c r="C33" s="38">
+      <c r="C33" s="13">
         <v>60</v>
       </c>
-      <c r="D33" s="38">
+      <c r="D33" s="13">
         <v>2.38</v>
       </c>
-      <c r="E33" s="38">
+      <c r="E33" s="13">
         <v>0.15</v>
       </c>
-      <c r="F33" s="38">
+      <c r="F33" s="13">
         <v>0</v>
       </c>
-      <c r="G33" s="38">
+      <c r="G33" s="13">
         <v>2000</v>
       </c>
-      <c r="H33" s="38">
+      <c r="H33" s="13">
         <v>100</v>
       </c>
-      <c r="I33" s="38">
+      <c r="I33" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A34" s="37" t="s">
+      <c r="A34" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="38">
+      <c r="B34" s="13">
         <v>25</v>
       </c>
-      <c r="C34" s="38">
+      <c r="C34" s="13">
         <v>60</v>
       </c>
-      <c r="D34" s="38">
+      <c r="D34" s="13">
         <v>2.38</v>
       </c>
-      <c r="E34" s="38">
+      <c r="E34" s="13">
         <v>0.15</v>
       </c>
-      <c r="F34" s="38">
+      <c r="F34" s="13">
         <v>0</v>
       </c>
-      <c r="G34" s="38">
+      <c r="G34" s="13">
         <v>2000</v>
       </c>
-      <c r="H34" s="38">
+      <c r="H34" s="13">
         <v>100</v>
       </c>
-      <c r="I34" s="38">
+      <c r="I34" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A35" s="37" t="s">
+      <c r="A35" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="38">
+      <c r="B35" s="13">
         <v>45</v>
       </c>
-      <c r="C35" s="38">
+      <c r="C35" s="13">
         <v>20</v>
       </c>
-      <c r="D35" s="38">
+      <c r="D35" s="13">
         <v>4</v>
       </c>
-      <c r="E35" s="38">
+      <c r="E35" s="13">
         <v>0.47</v>
       </c>
-      <c r="F35" s="38">
+      <c r="F35" s="13">
         <v>0</v>
       </c>
-      <c r="G35" s="38">
+      <c r="G35" s="13">
         <v>0.7</v>
       </c>
-      <c r="H35" s="38">
+      <c r="H35" s="13">
         <v>100</v>
       </c>
-      <c r="I35" s="38">
+      <c r="I35" s="13">
         <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A36" s="37" t="s">
+      <c r="A36" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="38">
+      <c r="B36" s="13">
         <v>45</v>
       </c>
-      <c r="C36" s="38">
+      <c r="C36" s="13">
         <v>20</v>
       </c>
-      <c r="D36" s="38">
+      <c r="D36" s="13">
         <v>4</v>
       </c>
-      <c r="E36" s="38">
+      <c r="E36" s="13">
         <v>0.47</v>
       </c>
-      <c r="F36" s="38">
+      <c r="F36" s="13">
         <v>0</v>
       </c>
-      <c r="G36" s="38">
+      <c r="G36" s="13">
         <v>2.6280000000000001</v>
       </c>
-      <c r="H36" s="38">
+      <c r="H36" s="13">
         <v>100</v>
       </c>
-      <c r="I36" s="38">
+      <c r="I36" s="13">
         <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A37" s="37" t="s">
+      <c r="A37" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="38">
+      <c r="B37" s="13">
         <v>45</v>
       </c>
-      <c r="C37" s="38">
+      <c r="C37" s="13">
         <v>20</v>
       </c>
-      <c r="D37" s="38">
+      <c r="D37" s="13">
         <v>4</v>
       </c>
-      <c r="E37" s="38">
+      <c r="E37" s="13">
         <v>0.22</v>
       </c>
-      <c r="F37" s="38">
+      <c r="F37" s="13">
         <v>0</v>
       </c>
-      <c r="G37" s="38">
+      <c r="G37" s="13">
         <v>3096</v>
       </c>
-      <c r="H37" s="38">
+      <c r="H37" s="13">
         <v>100</v>
       </c>
-      <c r="I37" s="38">
+      <c r="I37" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A38" s="37" t="s">
+      <c r="A38" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="38">
+      <c r="B38" s="13">
         <v>35</v>
       </c>
-      <c r="C38" s="38">
+      <c r="C38" s="13">
         <v>60</v>
       </c>
-      <c r="D38" s="38">
+      <c r="D38" s="13">
         <v>2</v>
       </c>
-      <c r="E38" s="38">
+      <c r="E38" s="13">
         <v>0.42</v>
       </c>
-      <c r="F38" s="38">
+      <c r="F38" s="13">
         <v>0</v>
       </c>
-      <c r="G38" s="38">
+      <c r="G38" s="13">
         <v>1.1100000000000001</v>
       </c>
-      <c r="H38" s="38">
+      <c r="H38" s="13">
         <v>100</v>
       </c>
-      <c r="I38" s="38">
+      <c r="I38" s="13">
         <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A39" s="37" t="s">
+      <c r="A39" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="38">
+      <c r="B39" s="13">
         <v>35</v>
       </c>
-      <c r="C39" s="38">
+      <c r="C39" s="13">
         <v>20</v>
       </c>
-      <c r="D39" s="38">
+      <c r="D39" s="13">
         <v>3</v>
       </c>
-      <c r="E39" s="38">
+      <c r="E39" s="13">
         <v>0.4</v>
       </c>
-      <c r="F39" s="38">
+      <c r="F39" s="13">
         <v>0</v>
       </c>
-      <c r="G39" s="38">
+      <c r="G39" s="13">
         <v>1.71</v>
       </c>
-      <c r="H39" s="38">
+      <c r="H39" s="13">
         <v>100</v>
       </c>
-      <c r="I39" s="38">
+      <c r="I39" s="13">
         <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="37" t="s">
+      <c r="A40" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="38">
+      <c r="B40" s="13">
         <v>35</v>
       </c>
-      <c r="C40" s="38">
+      <c r="C40" s="13">
         <v>90</v>
       </c>
-      <c r="D40" s="38">
+      <c r="D40" s="13">
         <v>2</v>
       </c>
-      <c r="E40" s="38">
+      <c r="E40" s="13">
         <v>0.38</v>
       </c>
-      <c r="F40" s="38">
+      <c r="F40" s="13">
         <v>0</v>
       </c>
-      <c r="G40" s="38">
+      <c r="G40" s="13">
         <v>3.46</v>
       </c>
-      <c r="H40" s="38">
+      <c r="H40" s="13">
         <v>100</v>
       </c>
-      <c r="I40" s="38">
+      <c r="I40" s="13">
         <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A41" s="37" t="s">
+      <c r="A41" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="38">
+      <c r="B41" s="13">
         <v>80</v>
       </c>
-      <c r="C41" s="38">
+      <c r="C41" s="13">
         <v>8</v>
       </c>
-      <c r="D41" s="38">
+      <c r="D41" s="13">
         <v>0.1</v>
       </c>
-      <c r="E41" s="38">
+      <c r="E41" s="13">
         <v>0.6</v>
       </c>
-      <c r="F41" s="38">
+      <c r="F41" s="13">
         <v>0</v>
       </c>
-      <c r="G41" s="38">
+      <c r="G41" s="13">
         <v>2.0299999999999998</v>
       </c>
-      <c r="H41" s="38">
+      <c r="H41" s="13">
         <v>100</v>
       </c>
-      <c r="I41" s="38">
+      <c r="I41" s="13">
         <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A42" s="37" t="s">
+      <c r="A42" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="38">
+      <c r="B42" s="13">
         <v>85</v>
       </c>
-      <c r="C42" s="38">
+      <c r="C42" s="13">
         <v>9</v>
       </c>
-      <c r="D42" s="38">
+      <c r="D42" s="13">
         <v>0.1</v>
       </c>
-      <c r="E42" s="38">
+      <c r="E42" s="13">
         <v>0.6</v>
       </c>
-      <c r="F42" s="38">
+      <c r="F42" s="13">
         <v>0</v>
       </c>
-      <c r="G42" s="38">
+      <c r="G42" s="13">
         <v>2.1</v>
       </c>
-      <c r="H42" s="38">
+      <c r="H42" s="13">
         <v>100</v>
       </c>
-      <c r="I42" s="38">
+      <c r="I42" s="13">
         <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A43" s="37" t="s">
+      <c r="A43" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="38">
+      <c r="B43" s="13">
         <v>80</v>
       </c>
-      <c r="C43" s="38">
+      <c r="C43" s="13">
         <v>9</v>
       </c>
-      <c r="D43" s="38">
+      <c r="D43" s="13">
         <v>0.1</v>
       </c>
-      <c r="E43" s="38">
+      <c r="E43" s="13">
         <v>0.6</v>
       </c>
-      <c r="F43" s="38">
+      <c r="F43" s="13">
         <v>0</v>
       </c>
-      <c r="G43" s="38">
+      <c r="G43" s="13">
         <v>2.4220000000000002</v>
       </c>
-      <c r="H43" s="38">
+      <c r="H43" s="13">
         <v>100</v>
       </c>
-      <c r="I43" s="38">
+      <c r="I43" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A44" s="37" t="s">
+      <c r="A44" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="38">
+      <c r="B44" s="13">
         <v>80</v>
       </c>
-      <c r="C44" s="38">
+      <c r="C44" s="13">
         <v>10</v>
       </c>
-      <c r="D44" s="38">
+      <c r="D44" s="13">
         <v>0.1</v>
       </c>
-      <c r="E44" s="38">
+      <c r="E44" s="13">
         <v>0.6</v>
       </c>
-      <c r="F44" s="38">
+      <c r="F44" s="13">
         <v>0</v>
       </c>
-      <c r="G44" s="38">
+      <c r="G44" s="13">
         <v>2.101</v>
       </c>
-      <c r="H44" s="38">
+      <c r="H44" s="13">
         <v>100</v>
       </c>
-      <c r="I44" s="38">
+      <c r="I44" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A45" s="37" t="s">
+      <c r="A45" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="38">
+      <c r="B45" s="13">
         <v>80</v>
       </c>
-      <c r="C45" s="38">
+      <c r="C45" s="13">
         <v>11</v>
       </c>
-      <c r="D45" s="38">
+      <c r="D45" s="13">
         <v>0.1</v>
       </c>
-      <c r="E45" s="38">
+      <c r="E45" s="13">
         <v>0.6</v>
       </c>
-      <c r="F45" s="38">
+      <c r="F45" s="13">
         <v>0</v>
       </c>
-      <c r="G45" s="38">
+      <c r="G45" s="13">
         <v>2.2690000000000001</v>
       </c>
-      <c r="H45" s="38">
+      <c r="H45" s="13">
         <v>100</v>
       </c>
-      <c r="I45" s="38">
+      <c r="I45" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A46" s="37" t="s">
+      <c r="A46" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="38">
+      <c r="B46" s="13">
         <v>80</v>
       </c>
-      <c r="C46" s="38">
+      <c r="C46" s="13">
         <v>12</v>
       </c>
-      <c r="D46" s="38">
+      <c r="D46" s="13">
         <v>0.1</v>
       </c>
-      <c r="E46" s="38">
+      <c r="E46" s="13">
         <v>0.6</v>
       </c>
-      <c r="F46" s="38">
+      <c r="F46" s="13">
         <v>0</v>
       </c>
-      <c r="G46" s="38">
+      <c r="G46" s="13">
         <v>1.7529999999999999</v>
       </c>
-      <c r="H46" s="38">
+      <c r="H46" s="13">
         <v>96.6</v>
       </c>
-      <c r="I46" s="38">
+      <c r="I46" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A47" s="37" t="s">
+      <c r="A47" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B47" s="38">
+      <c r="B47" s="13">
         <v>85</v>
       </c>
-      <c r="C47" s="38">
+      <c r="C47" s="13">
         <v>11</v>
       </c>
-      <c r="D47" s="38">
+      <c r="D47" s="13">
         <v>0.1</v>
       </c>
-      <c r="E47" s="38">
+      <c r="E47" s="13">
         <v>0.6</v>
       </c>
-      <c r="F47" s="38">
+      <c r="F47" s="13">
         <v>0</v>
       </c>
-      <c r="G47" s="38">
+      <c r="G47" s="13">
         <v>1.3320000000000001</v>
       </c>
-      <c r="H47" s="38">
+      <c r="H47" s="13">
         <v>98.8</v>
       </c>
-      <c r="I47" s="38">
+      <c r="I47" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A48" s="37" t="s">
+      <c r="A48" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B48" s="38">
+      <c r="B48" s="13">
         <v>88</v>
       </c>
-      <c r="C48" s="38">
+      <c r="C48" s="13">
         <v>9</v>
       </c>
-      <c r="D48" s="38">
+      <c r="D48" s="13">
         <v>0.1</v>
       </c>
-      <c r="E48" s="38">
+      <c r="E48" s="13">
         <v>0.6</v>
       </c>
-      <c r="F48" s="38">
+      <c r="F48" s="13">
         <v>0</v>
       </c>
-      <c r="G48" s="38">
+      <c r="G48" s="13">
         <v>2.496</v>
       </c>
-      <c r="H48" s="38">
+      <c r="H48" s="13">
         <v>100</v>
       </c>
-      <c r="I48" s="38">
+      <c r="I48" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A49" s="37" t="s">
+      <c r="A49" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B49" s="38">
+      <c r="B49" s="13">
         <v>88</v>
       </c>
-      <c r="C49" s="38">
+      <c r="C49" s="13">
         <v>10</v>
       </c>
-      <c r="D49" s="38">
+      <c r="D49" s="13">
         <v>0.1</v>
       </c>
-      <c r="E49" s="38">
+      <c r="E49" s="13">
         <v>0.6</v>
       </c>
-      <c r="F49" s="38">
+      <c r="F49" s="13">
         <v>0</v>
       </c>
-      <c r="G49" s="38">
+      <c r="G49" s="13">
         <v>2.3069999999999999</v>
       </c>
-      <c r="H49" s="38">
+      <c r="H49" s="13">
         <v>99.3</v>
       </c>
-      <c r="I49" s="38">
+      <c r="I49" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A50" s="37" t="s">
+      <c r="A50" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B50" s="38">
+      <c r="B50" s="13">
         <v>89</v>
       </c>
-      <c r="C50" s="38">
+      <c r="C50" s="13">
         <v>9</v>
       </c>
-      <c r="D50" s="38">
+      <c r="D50" s="13">
         <v>0.1</v>
       </c>
-      <c r="E50" s="38">
+      <c r="E50" s="13">
         <v>0.6</v>
       </c>
-      <c r="F50" s="38">
+      <c r="F50" s="13">
         <v>0</v>
       </c>
-      <c r="G50" s="38">
+      <c r="G50" s="13">
         <v>1.8779999999999999</v>
       </c>
-      <c r="H50" s="38">
+      <c r="H50" s="13">
         <v>100</v>
       </c>
-      <c r="I50" s="38">
+      <c r="I50" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A51" s="37" t="s">
+      <c r="A51" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B51" s="38">
+      <c r="B51" s="13">
         <v>89</v>
       </c>
-      <c r="C51" s="38">
+      <c r="C51" s="13">
         <v>10</v>
       </c>
-      <c r="D51" s="38">
+      <c r="D51" s="13">
         <v>0.1</v>
       </c>
-      <c r="E51" s="38">
+      <c r="E51" s="13">
         <v>0.6</v>
       </c>
-      <c r="F51" s="38">
+      <c r="F51" s="13">
         <v>0</v>
       </c>
-      <c r="G51" s="38">
+      <c r="G51" s="13">
         <v>2.069</v>
       </c>
-      <c r="H51" s="38">
+      <c r="H51" s="13">
         <v>100</v>
       </c>
-      <c r="I51" s="38">
+      <c r="I51" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A52" s="37" t="s">
+      <c r="A52" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B52" s="38">
+      <c r="B52" s="13">
         <v>93</v>
       </c>
-      <c r="C52" s="38">
+      <c r="C52" s="13">
         <v>11</v>
       </c>
-      <c r="D52" s="38">
+      <c r="D52" s="13">
         <v>0.1</v>
       </c>
-      <c r="E52" s="38">
+      <c r="E52" s="13">
         <v>0.6</v>
       </c>
-      <c r="F52" s="38">
+      <c r="F52" s="13">
         <v>0</v>
       </c>
-      <c r="G52" s="38">
+      <c r="G52" s="13">
         <v>2.7629999999999999</v>
       </c>
-      <c r="H52" s="38">
+      <c r="H52" s="13">
         <v>100</v>
       </c>
-      <c r="I52" s="38">
+      <c r="I52" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A53" s="37" t="s">
+      <c r="A53" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B53" s="38">
+      <c r="B53" s="13">
         <v>93</v>
       </c>
-      <c r="C53" s="38">
+      <c r="C53" s="13">
         <v>12</v>
       </c>
-      <c r="D53" s="38">
+      <c r="D53" s="13">
         <v>0.1</v>
       </c>
-      <c r="E53" s="38">
+      <c r="E53" s="13">
         <v>0.6</v>
       </c>
-      <c r="F53" s="38">
+      <c r="F53" s="13">
         <v>0</v>
       </c>
-      <c r="G53" s="38">
+      <c r="G53" s="13">
         <v>3.2189999999999999</v>
       </c>
-      <c r="H53" s="38">
+      <c r="H53" s="13">
         <v>99.7</v>
       </c>
-      <c r="I53" s="38">
+      <c r="I53" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A54" s="37" t="s">
+      <c r="A54" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B54" s="38">
+      <c r="B54" s="13">
         <v>71</v>
       </c>
-      <c r="C54" s="38">
+      <c r="C54" s="13">
         <v>9</v>
       </c>
-      <c r="D54" s="38">
+      <c r="D54" s="13">
         <v>0.1</v>
       </c>
-      <c r="E54" s="38">
+      <c r="E54" s="13">
         <v>0.6</v>
       </c>
-      <c r="F54" s="38">
+      <c r="F54" s="13">
         <v>0</v>
       </c>
-      <c r="G54" s="38">
+      <c r="G54" s="13">
         <v>1.893</v>
       </c>
-      <c r="H54" s="38">
+      <c r="H54" s="13">
         <v>100</v>
       </c>
-      <c r="I54" s="38">
+      <c r="I54" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A55" s="37" t="s">
+      <c r="A55" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B55" s="38">
+      <c r="B55" s="13">
         <v>71</v>
       </c>
-      <c r="C55" s="38">
+      <c r="C55" s="13">
         <v>9</v>
       </c>
-      <c r="D55" s="38">
+      <c r="D55" s="13">
         <v>0.1</v>
       </c>
-      <c r="E55" s="38">
+      <c r="E55" s="13">
         <v>0.6</v>
       </c>
-      <c r="F55" s="38">
+      <c r="F55" s="13">
         <v>0.5</v>
       </c>
-      <c r="G55" s="38">
+      <c r="G55" s="13">
         <v>1.9670000000000001</v>
       </c>
-      <c r="H55" s="38">
+      <c r="H55" s="13">
         <v>100</v>
       </c>
-      <c r="I55" s="38">
+      <c r="I55" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A56" s="37" t="s">
+      <c r="A56" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B56" s="38">
+      <c r="B56" s="13">
         <v>71</v>
       </c>
-      <c r="C56" s="38">
+      <c r="C56" s="13">
         <v>9</v>
       </c>
-      <c r="D56" s="38">
+      <c r="D56" s="13">
         <v>0.1</v>
       </c>
-      <c r="E56" s="38">
+      <c r="E56" s="13">
         <v>0.6</v>
       </c>
-      <c r="F56" s="38">
+      <c r="F56" s="13">
         <v>1</v>
       </c>
-      <c r="G56" s="38">
+      <c r="G56" s="13">
         <v>2.1219999999999999</v>
       </c>
-      <c r="H56" s="38">
+      <c r="H56" s="13">
         <v>100</v>
       </c>
-      <c r="I56" s="38">
+      <c r="I56" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A57" s="37" t="s">
+      <c r="A57" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B57" s="38">
+      <c r="B57" s="13">
         <v>71</v>
       </c>
-      <c r="C57" s="38">
+      <c r="C57" s="13">
         <v>9</v>
       </c>
-      <c r="D57" s="38">
+      <c r="D57" s="13">
         <v>0.1</v>
       </c>
-      <c r="E57" s="38">
+      <c r="E57" s="13">
         <v>0.6</v>
       </c>
-      <c r="F57" s="38">
-        <v>45047</v>
-      </c>
-      <c r="G57" s="38">
+      <c r="F57" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="G57" s="13">
         <v>1.784</v>
       </c>
-      <c r="H57" s="38">
+      <c r="H57" s="13">
         <v>100</v>
       </c>
-      <c r="I57" s="38">
+      <c r="I57" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A58" s="37" t="s">
+      <c r="A58" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B58" s="38">
+      <c r="B58" s="13">
         <v>71</v>
       </c>
-      <c r="C58" s="38">
+      <c r="C58" s="13">
         <v>10</v>
       </c>
-      <c r="D58" s="38">
+      <c r="D58" s="13">
         <v>0.1</v>
       </c>
-      <c r="E58" s="38">
+      <c r="E58" s="13">
         <v>0.6</v>
       </c>
-      <c r="F58" s="38">
+      <c r="F58" s="13">
         <v>0</v>
       </c>
-      <c r="G58" s="38">
+      <c r="G58" s="13">
         <v>1.958</v>
       </c>
-      <c r="H58" s="38">
+      <c r="H58" s="13">
         <v>100</v>
       </c>
-      <c r="I58" s="38">
+      <c r="I58" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A59" s="37" t="s">
+      <c r="A59" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B59" s="38">
+      <c r="B59" s="13">
         <v>71</v>
       </c>
-      <c r="C59" s="38">
+      <c r="C59" s="13">
         <v>10</v>
       </c>
-      <c r="D59" s="38">
+      <c r="D59" s="13">
         <v>0.1</v>
       </c>
-      <c r="E59" s="38">
+      <c r="E59" s="13">
         <v>0.6</v>
       </c>
-      <c r="F59" s="38">
+      <c r="F59" s="13">
         <v>0.5</v>
       </c>
-      <c r="G59" s="38">
+      <c r="G59" s="13">
         <v>1.9379999999999999</v>
       </c>
-      <c r="H59" s="38">
+      <c r="H59" s="13">
         <v>100</v>
       </c>
-      <c r="I59" s="38">
+      <c r="I59" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A60" s="37" t="s">
+      <c r="A60" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B60" s="38">
+      <c r="B60" s="13">
         <v>71</v>
       </c>
-      <c r="C60" s="38">
+      <c r="C60" s="13">
         <v>10</v>
       </c>
-      <c r="D60" s="38">
+      <c r="D60" s="13">
         <v>0.1</v>
       </c>
-      <c r="E60" s="38">
+      <c r="E60" s="13">
         <v>0.6</v>
       </c>
-      <c r="F60" s="38">
+      <c r="F60" s="13">
         <v>1</v>
       </c>
-      <c r="G60" s="38">
+      <c r="G60" s="13">
         <v>2.1869999999999998</v>
       </c>
-      <c r="H60" s="38">
+      <c r="H60" s="13">
         <v>100</v>
       </c>
-      <c r="I60" s="38">
+      <c r="I60" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A61" s="37" t="s">
+      <c r="A61" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B61" s="38">
+      <c r="B61" s="13">
         <v>71</v>
       </c>
-      <c r="C61" s="38">
+      <c r="C61" s="13">
         <v>10</v>
       </c>
-      <c r="D61" s="38">
+      <c r="D61" s="13">
         <v>0.1</v>
       </c>
-      <c r="E61" s="38">
+      <c r="E61" s="13">
         <v>0.6</v>
       </c>
-      <c r="F61" s="38">
-        <v>45047</v>
-      </c>
-      <c r="G61" s="38">
+      <c r="F61" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="G61" s="13">
         <v>2.0859999999999999</v>
       </c>
-      <c r="H61" s="38">
+      <c r="H61" s="13">
         <v>100</v>
       </c>
-      <c r="I61" s="38">
+      <c r="I61" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A62" s="37" t="s">
+      <c r="A62" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B62" s="38">
+      <c r="B62" s="13">
         <v>71</v>
       </c>
-      <c r="C62" s="38">
+      <c r="C62" s="13">
         <v>11</v>
       </c>
-      <c r="D62" s="38">
+      <c r="D62" s="13">
         <v>0.1</v>
       </c>
-      <c r="E62" s="38">
+      <c r="E62" s="13">
         <v>0.6</v>
       </c>
-      <c r="F62" s="38">
+      <c r="F62" s="13">
         <v>0</v>
       </c>
-      <c r="G62" s="38">
+      <c r="G62" s="13">
         <v>2.1760000000000002</v>
       </c>
-      <c r="H62" s="38">
+      <c r="H62" s="13">
         <v>100</v>
       </c>
-      <c r="I62" s="38">
+      <c r="I62" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A63" s="37" t="s">
+      <c r="A63" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B63" s="38">
+      <c r="B63" s="13">
         <v>71</v>
       </c>
-      <c r="C63" s="38">
+      <c r="C63" s="13">
         <v>11</v>
       </c>
-      <c r="D63" s="38">
+      <c r="D63" s="13">
         <v>0.1</v>
       </c>
-      <c r="E63" s="38">
+      <c r="E63" s="13">
         <v>0.6</v>
       </c>
-      <c r="F63" s="38">
+      <c r="F63" s="13">
         <v>0.5</v>
       </c>
-      <c r="G63" s="38">
+      <c r="G63" s="13">
         <v>2.2160000000000002</v>
       </c>
-      <c r="H63" s="38">
+      <c r="H63" s="13">
         <v>100</v>
       </c>
-      <c r="I63" s="38">
+      <c r="I63" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A64" s="37" t="s">
+      <c r="A64" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B64" s="38">
+      <c r="B64" s="13">
         <v>71</v>
       </c>
-      <c r="C64" s="38">
+      <c r="C64" s="13">
         <v>11</v>
       </c>
-      <c r="D64" s="38">
+      <c r="D64" s="13">
         <v>0.1</v>
       </c>
-      <c r="E64" s="38">
+      <c r="E64" s="13">
         <v>0.6</v>
       </c>
-      <c r="F64" s="38">
+      <c r="F64" s="13">
         <v>1</v>
       </c>
-      <c r="G64" s="38">
+      <c r="G64" s="13">
         <v>2.0169999999999999</v>
       </c>
-      <c r="H64" s="38">
+      <c r="H64" s="13">
         <v>100</v>
       </c>
-      <c r="I64" s="38">
+      <c r="I64" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A65" s="37" t="s">
+      <c r="A65" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B65" s="38">
+      <c r="B65" s="13">
         <v>71</v>
       </c>
-      <c r="C65" s="38">
+      <c r="C65" s="13">
         <v>11</v>
       </c>
-      <c r="D65" s="38">
+      <c r="D65" s="13">
         <v>0.1</v>
       </c>
-      <c r="E65" s="38">
+      <c r="E65" s="13">
         <v>0.6</v>
       </c>
-      <c r="F65" s="38">
-        <v>45047</v>
-      </c>
-      <c r="G65" s="38">
+      <c r="F65" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="G65" s="13">
         <v>2.2549999999999999</v>
       </c>
-      <c r="H65" s="38">
+      <c r="H65" s="13">
         <v>100</v>
       </c>
-      <c r="I65" s="38">
+      <c r="I65" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A66" s="37" t="s">
+      <c r="A66" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B66" s="38">
+      <c r="B66" s="13">
         <v>71</v>
       </c>
-      <c r="C66" s="38">
+      <c r="C66" s="13">
         <v>12</v>
       </c>
-      <c r="D66" s="38">
+      <c r="D66" s="13">
         <v>0.1</v>
       </c>
-      <c r="E66" s="38">
+      <c r="E66" s="13">
         <v>0.6</v>
       </c>
-      <c r="F66" s="38">
+      <c r="F66" s="13">
         <v>0</v>
       </c>
-      <c r="G66" s="38">
+      <c r="G66" s="13">
         <v>2.1850000000000001</v>
       </c>
-      <c r="H66" s="38">
+      <c r="H66" s="13">
         <v>100</v>
       </c>
-      <c r="I66" s="38">
+      <c r="I66" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A67" s="37" t="s">
+      <c r="A67" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B67" s="38">
+      <c r="B67" s="13">
         <v>71</v>
       </c>
-      <c r="C67" s="38">
+      <c r="C67" s="13">
         <v>12</v>
       </c>
-      <c r="D67" s="38">
+      <c r="D67" s="13">
         <v>0.1</v>
       </c>
-      <c r="E67" s="38">
+      <c r="E67" s="13">
         <v>0.6</v>
       </c>
-      <c r="F67" s="38">
+      <c r="F67" s="13">
         <v>0.5</v>
       </c>
-      <c r="G67" s="38">
+      <c r="G67" s="13">
         <v>1.9810000000000001</v>
       </c>
-      <c r="H67" s="38">
+      <c r="H67" s="13">
         <v>100</v>
       </c>
-      <c r="I67" s="38">
+      <c r="I67" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A68" s="37" t="s">
+      <c r="A68" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B68" s="38">
+      <c r="B68" s="13">
         <v>71</v>
       </c>
-      <c r="C68" s="38">
+      <c r="C68" s="13">
         <v>12</v>
       </c>
-      <c r="D68" s="38">
+      <c r="D68" s="13">
         <v>0.1</v>
       </c>
-      <c r="E68" s="38">
+      <c r="E68" s="13">
         <v>0.6</v>
       </c>
-      <c r="F68" s="38">
+      <c r="F68" s="13">
         <v>1</v>
       </c>
-      <c r="G68" s="38">
+      <c r="G68" s="13">
         <v>1.762</v>
       </c>
-      <c r="H68" s="38">
+      <c r="H68" s="13">
         <v>100</v>
       </c>
-      <c r="I68" s="38">
+      <c r="I68" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A69" s="37" t="s">
+      <c r="A69" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B69" s="38">
+      <c r="B69" s="13">
         <v>71</v>
       </c>
-      <c r="C69" s="38">
+      <c r="C69" s="13">
         <v>12</v>
       </c>
-      <c r="D69" s="38">
+      <c r="D69" s="13">
         <v>0.1</v>
       </c>
-      <c r="E69" s="38">
+      <c r="E69" s="13">
         <v>0.6</v>
       </c>
-      <c r="F69" s="38">
-        <v>45047</v>
-      </c>
-      <c r="G69" s="38">
+      <c r="F69" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="G69" s="13">
         <v>2.0219999999999998</v>
       </c>
-      <c r="H69" s="38">
+      <c r="H69" s="13">
         <v>100</v>
       </c>
-      <c r="I69" s="38">
+      <c r="I69" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A70" s="37" t="s">
+      <c r="A70" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B70" s="38">
+      <c r="B70" s="13">
         <v>65</v>
       </c>
-      <c r="C70" s="38">
+      <c r="C70" s="13">
         <v>12</v>
       </c>
-      <c r="D70" s="38">
+      <c r="D70" s="13">
         <v>0.1</v>
       </c>
-      <c r="E70" s="38">
+      <c r="E70" s="13">
         <v>0.6</v>
       </c>
-      <c r="F70" s="38">
+      <c r="F70" s="13">
         <v>0</v>
       </c>
-      <c r="G70" s="38">
+      <c r="G70" s="13">
         <v>1.377</v>
       </c>
-      <c r="H70" s="38">
+      <c r="H70" s="13">
         <v>97.5</v>
       </c>
-      <c r="I70" s="38">
+      <c r="I70" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A71" s="37" t="s">
+      <c r="A71" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B71" s="38">
+      <c r="B71" s="13">
         <v>75</v>
       </c>
-      <c r="C71" s="38">
+      <c r="C71" s="13">
         <v>12</v>
       </c>
-      <c r="D71" s="38">
+      <c r="D71" s="13">
         <v>0.1</v>
       </c>
-      <c r="E71" s="38">
+      <c r="E71" s="13">
         <v>0.6</v>
       </c>
-      <c r="F71" s="38">
+      <c r="F71" s="13">
         <v>0</v>
       </c>
-      <c r="G71" s="38">
+      <c r="G71" s="13">
         <v>3.3039999999999998</v>
       </c>
-      <c r="H71" s="38">
+      <c r="H71" s="13">
         <v>100</v>
       </c>
-      <c r="I71" s="38">
+      <c r="I71" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A72" s="37" t="s">
+      <c r="A72" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B72" s="38">
+      <c r="B72" s="13">
         <v>85</v>
       </c>
-      <c r="C72" s="38">
+      <c r="C72" s="13">
         <v>12</v>
       </c>
-      <c r="D72" s="38">
+      <c r="D72" s="13">
         <v>0.1</v>
       </c>
-      <c r="E72" s="38">
+      <c r="E72" s="13">
         <v>0.6</v>
       </c>
-      <c r="F72" s="38">
+      <c r="F72" s="13">
         <v>0</v>
       </c>
-      <c r="G72" s="38">
+      <c r="G72" s="13">
         <v>2000</v>
       </c>
-      <c r="H72" s="38">
+      <c r="H72" s="13">
         <v>100</v>
       </c>
-      <c r="I72" s="38">
+      <c r="I72" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A73" s="37" t="s">
+      <c r="A73" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B73" s="38">
+      <c r="B73" s="13">
         <v>70</v>
       </c>
-      <c r="C73" s="38">
+      <c r="C73" s="13">
         <v>12</v>
       </c>
-      <c r="D73" s="38">
+      <c r="D73" s="13">
         <v>0.1</v>
       </c>
-      <c r="E73" s="38">
+      <c r="E73" s="13">
         <v>0.62</v>
       </c>
-      <c r="F73" s="38">
+      <c r="F73" s="13">
         <v>0</v>
       </c>
-      <c r="G73" s="38">
+      <c r="G73" s="13">
         <v>2.9</v>
       </c>
-      <c r="H73" s="38">
+      <c r="H73" s="13">
         <v>99.5</v>
       </c>
-      <c r="I73" s="38">
+      <c r="I73" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A74" s="37" t="s">
+      <c r="A74" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B74" s="38">
+      <c r="B74" s="13">
         <v>70</v>
       </c>
-      <c r="C74" s="38">
+      <c r="C74" s="13">
         <v>12</v>
       </c>
-      <c r="D74" s="38">
+      <c r="D74" s="13">
         <v>0.1</v>
       </c>
-      <c r="E74" s="38">
+      <c r="E74" s="13">
         <v>0.59</v>
       </c>
-      <c r="F74" s="38">
+      <c r="F74" s="13">
         <v>0</v>
       </c>
-      <c r="G74" s="38">
+      <c r="G74" s="13">
         <v>1.901</v>
       </c>
-      <c r="H74" s="38">
+      <c r="H74" s="13">
         <v>100</v>
       </c>
-      <c r="I74" s="38">
+      <c r="I74" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A75" s="37" t="s">
+      <c r="A75" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B75" s="38">
+      <c r="B75" s="13">
         <v>70</v>
       </c>
-      <c r="C75" s="38">
+      <c r="C75" s="13">
         <v>12</v>
       </c>
-      <c r="D75" s="38">
+      <c r="D75" s="13">
         <v>0.1</v>
       </c>
-      <c r="E75" s="38">
+      <c r="E75" s="13">
         <v>0.55000000000000004</v>
       </c>
-      <c r="F75" s="38">
+      <c r="F75" s="13">
         <v>0</v>
       </c>
-      <c r="G75" s="38">
+      <c r="G75" s="13">
         <v>2.8410000000000002</v>
       </c>
-      <c r="H75" s="38">
+      <c r="H75" s="13">
         <v>100</v>
       </c>
-      <c r="I75" s="38">
+      <c r="I75" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A76" s="37" t="s">
+      <c r="A76" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B76" s="38">
+      <c r="B76" s="13">
         <v>70</v>
       </c>
-      <c r="C76" s="38">
+      <c r="C76" s="13">
         <v>12</v>
       </c>
-      <c r="D76" s="38">
+      <c r="D76" s="13">
         <v>0.1</v>
       </c>
-      <c r="E76" s="38">
+      <c r="E76" s="13">
         <v>0.52</v>
       </c>
-      <c r="F76" s="38">
+      <c r="F76" s="13">
         <v>0</v>
       </c>
-      <c r="G76" s="38">
+      <c r="G76" s="13">
         <v>2.1619999999999999</v>
       </c>
-      <c r="H76" s="38">
+      <c r="H76" s="13">
         <v>97.8</v>
       </c>
-      <c r="I76" s="38">
+      <c r="I76" s="13">
         <v>40</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A77" s="37" t="s">
+      <c r="A77" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B77" s="38">
+      <c r="B77" s="13">
         <v>80</v>
       </c>
-      <c r="C77" s="38">
+      <c r="C77" s="13">
         <v>8</v>
       </c>
-      <c r="D77" s="38">
+      <c r="D77" s="13">
         <v>0.1</v>
       </c>
-      <c r="E77" s="38">
+      <c r="E77" s="13">
         <v>0.6</v>
       </c>
-      <c r="F77" s="38">
+      <c r="F77" s="13">
         <v>0</v>
       </c>
-      <c r="G77" s="38">
+      <c r="G77" s="13">
         <v>2.1970000000000001</v>
       </c>
-      <c r="H77" s="38">
+      <c r="H77" s="13">
         <v>100</v>
       </c>
-      <c r="I77" s="38">
+      <c r="I77" s="13">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add 3 stage for titan sole
</commit_message>
<xml_diff>
--- a/static/mock/titanium sols.xlsx
+++ b/static/mock/titanium sols.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexglushko/ProgProjects/ChemML/static/mock/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexglushko/ProgramProj/ChemML/static/mock/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC02E81-6B58-3947-84B7-A40AF941092A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8DA4E7-470A-1446-A4F1-3954D4A8376C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{DA8300D2-1843-2443-8DD6-A95A819FF1FD}"/>
+    <workbookView xWindow="51200" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="3" xr2:uid="{DA8300D2-1843-2443-8DD6-A95A819FF1FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Experiment_data" sheetId="2" r:id="rId2"/>
     <sheet name="Experiment_data_2" sheetId="3" r:id="rId3"/>
+    <sheet name="Experiment_data_3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="151">
   <si>
     <t>Состав реакционных смесей</t>
   </si>
@@ -935,6 +936,9 @@
   </si>
   <si>
     <t xml:space="preserve">ultrasound </t>
+  </si>
+  <si>
+    <t>с(Ti4+), mol/l</t>
   </si>
 </sst>
 </file>
@@ -1179,7 +1183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1226,6 +1230,30 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1256,35 +1284,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1469,7 +1479,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1489,7 +1499,7 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1711,20 +1721,37 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1E371E53-33CA-5E40-8040-CB9EEA4707B2}" name="Table2" displayName="Table2" ref="A1:I77" totalsRowShown="0" headerRowDxfId="10" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1E371E53-33CA-5E40-8040-CB9EEA4707B2}" name="Table2" displayName="Table2" ref="A1:I77" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:I77" xr:uid="{1E371E53-33CA-5E40-8040-CB9EEA4707B2}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{3FA7475C-433E-6D4F-B57A-00C1A515C892}" name="Composition mixtures" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{0F31B1B3-D1B1-EC4C-878B-D3AEADD20086}" name="t, °С" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{F3ADAC69-E7B8-474D-9047-06DDE55033C0}" name="t, min" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{981058E4-041A-3443-B21D-0F308E0A9A65}" name="с(acid), mol/l" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{EDCF82FF-93B9-8F4E-9258-5FC84BEFCAD0}" name="с(Ti4+), mol/l" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{43124716-5761-FA4D-B524-75FDAE619C96}" name="ultrasound " dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{C2FD9190-F3B5-6648-9534-696937C89906}" name="d, nm" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{805965AA-F35C-A949-966E-68FDEE7D2000}" name="Contents, %" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{9E1B3A05-9B84-2B4D-8FEE-A7940178837F}" name="Stability of sols, days" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{3FA7475C-433E-6D4F-B57A-00C1A515C892}" name="Composition mixtures" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{0F31B1B3-D1B1-EC4C-878B-D3AEADD20086}" name="t, °С" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{F3ADAC69-E7B8-474D-9047-06DDE55033C0}" name="t, min" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{981058E4-041A-3443-B21D-0F308E0A9A65}" name="с(acid), mol/l" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{EDCF82FF-93B9-8F4E-9258-5FC84BEFCAD0}" name="с(Ti4+), mol/l" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{43124716-5761-FA4D-B524-75FDAE619C96}" name="ultrasound " dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{C2FD9190-F3B5-6648-9534-696937C89906}" name="d, nm" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{805965AA-F35C-A949-966E-68FDEE7D2000}" name="Contents, %" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{9E1B3A05-9B84-2B4D-8FEE-A7940178837F}" name="Stability of sols, days" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{ED27386F-1021-0741-91AB-D2F5FCB3B5EE}" name="Table3" displayName="Table3" ref="A1:H65" totalsRowShown="0">
+  <autoFilter ref="A1:H65" xr:uid="{ED27386F-1021-0741-91AB-D2F5FCB3B5EE}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{D7F13098-9CED-CB48-AA54-91FF6A3AEDA1}" name="Composition mixtures"/>
+    <tableColumn id="2" xr3:uid="{6E653FBD-8806-0A4C-ABAD-CF69F33C077B}" name="t, °С"/>
+    <tableColumn id="3" xr3:uid="{8792B81C-9998-BE43-8ECF-E1D7509301D7}" name="t, min"/>
+    <tableColumn id="4" xr3:uid="{DA64BD69-E527-CF4B-B71C-48C06A8A6E0C}" name="с(acid), mol/l"/>
+    <tableColumn id="5" xr3:uid="{89F4369C-973C-5041-B1A8-FC50FA43FDBF}" name="с(Ti4+), mol/l"/>
+    <tableColumn id="7" xr3:uid="{1E12F946-D252-7E45-99E3-C7C91210D4B2}" name="d, nm"/>
+    <tableColumn id="8" xr3:uid="{DD4FD3FF-403E-EB43-ACD3-588028876B19}" name="Contents, %"/>
+    <tableColumn id="9" xr3:uid="{1EC95E20-297B-B94B-AFF2-F97423B1FE38}" name="Stability of sols, days"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -2034,67 +2061,67 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="22" t="s">
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="16" t="s">
+      <c r="H1" s="31"/>
+      <c r="I1" s="24" t="s">
         <v>3</v>
       </c>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="26" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="34" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="17"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="25"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="29"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="35"/>
       <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
       <c r="G3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="18"/>
+      <c r="I3" s="26"/>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="20" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="3">
@@ -2124,7 +2151,7 @@
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="3">
         <v>80</v>
       </c>
@@ -2152,7 +2179,7 @@
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="3">
         <v>45</v>
       </c>
@@ -2180,7 +2207,7 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="3">
         <v>45</v>
       </c>
@@ -2208,7 +2235,7 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="20" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="3">
@@ -2238,7 +2265,7 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="3">
         <v>50</v>
       </c>
@@ -2266,7 +2293,7 @@
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="3">
         <v>80</v>
       </c>
@@ -2294,7 +2321,7 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="3">
         <v>45</v>
       </c>
@@ -2322,7 +2349,7 @@
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="3">
         <v>60</v>
       </c>
@@ -2350,7 +2377,7 @@
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="3">
         <v>60</v>
       </c>
@@ -2378,20 +2405,20 @@
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="31"/>
-      <c r="B14" s="26">
+      <c r="A14" s="21"/>
+      <c r="B14" s="20">
         <v>45</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="20">
         <v>130</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="26" t="s">
+      <c r="E14" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="26" t="s">
+      <c r="F14" s="20" t="s">
         <v>14</v>
       </c>
       <c r="G14" s="6">
@@ -2400,29 +2427,29 @@
       <c r="H14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="26">
+      <c r="I14" s="20">
         <v>9</v>
       </c>
-      <c r="J14" s="30"/>
+      <c r="J14" s="23"/>
     </row>
     <row r="15" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
       <c r="G15" s="5">
         <v>45006</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="27"/>
-      <c r="J15" s="30"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="23"/>
     </row>
     <row r="16" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="3">
         <v>45</v>
       </c>
@@ -2450,7 +2477,7 @@
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="3">
         <v>25</v>
       </c>
@@ -2478,7 +2505,7 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="3">
         <v>45</v>
       </c>
@@ -2506,7 +2533,7 @@
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
+      <c r="A19" s="21"/>
       <c r="B19" s="3">
         <v>25</v>
       </c>
@@ -2534,7 +2561,7 @@
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="3">
         <v>20</v>
       </c>
@@ -2562,7 +2589,7 @@
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="3">
         <v>80</v>
       </c>
@@ -2590,7 +2617,7 @@
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="3">
         <v>45</v>
       </c>
@@ -2618,22 +2645,22 @@
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="26">
+      <c r="B23" s="20">
         <v>50</v>
       </c>
-      <c r="C23" s="26">
+      <c r="C23" s="20">
         <v>30</v>
       </c>
-      <c r="D23" s="26">
+      <c r="D23" s="20">
         <v>4</v>
       </c>
-      <c r="E23" s="26" t="s">
+      <c r="E23" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="26" t="s">
+      <c r="F23" s="20" t="s">
         <v>14</v>
       </c>
       <c r="G23" s="2">
@@ -2642,29 +2669,29 @@
       <c r="H23" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I23" s="26">
+      <c r="I23" s="20">
         <v>17</v>
       </c>
-      <c r="J23" s="30"/>
+      <c r="J23" s="23"/>
     </row>
     <row r="24" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="31"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
       <c r="G24" s="3" t="s">
         <v>35</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I24" s="27"/>
-      <c r="J24" s="30"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="23"/>
     </row>
     <row r="25" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="31"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="3">
         <v>80</v>
       </c>
@@ -2692,7 +2719,7 @@
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="3">
         <v>45</v>
       </c>
@@ -2720,7 +2747,7 @@
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="3">
         <v>60</v>
       </c>
@@ -2748,7 +2775,7 @@
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="3">
         <v>60</v>
       </c>
@@ -2776,7 +2803,7 @@
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="31"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="3">
         <v>60</v>
       </c>
@@ -2804,7 +2831,7 @@
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="31"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="3">
         <v>80</v>
       </c>
@@ -2832,7 +2859,7 @@
       <c r="J30" s="1"/>
     </row>
     <row r="31" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="3">
         <v>60</v>
       </c>
@@ -2860,7 +2887,7 @@
       <c r="J31" s="1"/>
     </row>
     <row r="32" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
+      <c r="A32" s="21"/>
       <c r="B32" s="3">
         <v>45</v>
       </c>
@@ -2888,7 +2915,7 @@
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="31"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="3">
         <v>20</v>
       </c>
@@ -2916,7 +2943,7 @@
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="31"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="3">
         <v>20</v>
       </c>
@@ -2944,7 +2971,7 @@
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="31"/>
+      <c r="A35" s="21"/>
       <c r="B35" s="3">
         <v>20</v>
       </c>
@@ -2972,7 +2999,7 @@
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="31"/>
+      <c r="A36" s="21"/>
       <c r="B36" s="3">
         <v>25</v>
       </c>
@@ -3000,7 +3027,7 @@
       <c r="J36" s="1"/>
     </row>
     <row r="37" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="31"/>
+      <c r="A37" s="21"/>
       <c r="B37" s="3">
         <v>45</v>
       </c>
@@ -3028,7 +3055,7 @@
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="27"/>
+      <c r="A38" s="22"/>
       <c r="B38" s="3">
         <v>45</v>
       </c>
@@ -3056,7 +3083,7 @@
       <c r="J38" s="1"/>
     </row>
     <row r="39" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="26" t="s">
+      <c r="A39" s="20" t="s">
         <v>43</v>
       </c>
       <c r="B39" s="3">
@@ -3086,7 +3113,7 @@
       <c r="J39" s="1"/>
     </row>
     <row r="40" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="31"/>
+      <c r="A40" s="21"/>
       <c r="B40" s="8">
         <v>80</v>
       </c>
@@ -3114,7 +3141,7 @@
       <c r="J40" s="1"/>
     </row>
     <row r="41" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="31"/>
+      <c r="A41" s="21"/>
       <c r="B41" s="8">
         <v>80</v>
       </c>
@@ -3142,7 +3169,7 @@
       <c r="J41" s="1"/>
     </row>
     <row r="42" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="31"/>
+      <c r="A42" s="21"/>
       <c r="B42" s="8">
         <v>80</v>
       </c>
@@ -3170,7 +3197,7 @@
       <c r="J42" s="1"/>
     </row>
     <row r="43" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="31"/>
+      <c r="A43" s="21"/>
       <c r="B43" s="8">
         <v>80</v>
       </c>
@@ -3198,7 +3225,7 @@
       <c r="J43" s="1"/>
     </row>
     <row r="44" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="31"/>
+      <c r="A44" s="21"/>
       <c r="B44" s="8">
         <v>85</v>
       </c>
@@ -3226,7 +3253,7 @@
       <c r="J44" s="1"/>
     </row>
     <row r="45" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="31"/>
+      <c r="A45" s="21"/>
       <c r="B45" s="8">
         <v>88</v>
       </c>
@@ -3254,7 +3281,7 @@
       <c r="J45" s="1"/>
     </row>
     <row r="46" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="31"/>
+      <c r="A46" s="21"/>
       <c r="B46" s="8">
         <v>88</v>
       </c>
@@ -3282,7 +3309,7 @@
       <c r="J46" s="1"/>
     </row>
     <row r="47" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="31"/>
+      <c r="A47" s="21"/>
       <c r="B47" s="8">
         <v>89</v>
       </c>
@@ -3310,7 +3337,7 @@
       <c r="J47" s="1"/>
     </row>
     <row r="48" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="31"/>
+      <c r="A48" s="21"/>
       <c r="B48" s="8">
         <v>89</v>
       </c>
@@ -3338,7 +3365,7 @@
       <c r="J48" s="1"/>
     </row>
     <row r="49" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="31"/>
+      <c r="A49" s="21"/>
       <c r="B49" s="8">
         <v>93</v>
       </c>
@@ -3366,7 +3393,7 @@
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="31"/>
+      <c r="A50" s="21"/>
       <c r="B50" s="8">
         <v>93</v>
       </c>
@@ -3394,17 +3421,17 @@
       <c r="J50" s="1"/>
     </row>
     <row r="51" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="31"/>
-      <c r="B51" s="32">
+      <c r="A51" s="21"/>
+      <c r="B51" s="17">
         <v>71</v>
       </c>
-      <c r="C51" s="32">
+      <c r="C51" s="17">
         <v>9</v>
       </c>
-      <c r="D51" s="32" t="s">
+      <c r="D51" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E51" s="32" t="s">
+      <c r="E51" s="17" t="s">
         <v>44</v>
       </c>
       <c r="F51" s="8" t="s">
@@ -3422,11 +3449,11 @@
       <c r="J51" s="1"/>
     </row>
     <row r="52" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="31"/>
-      <c r="B52" s="33"/>
-      <c r="C52" s="33"/>
-      <c r="D52" s="33"/>
-      <c r="E52" s="33"/>
+      <c r="A52" s="21"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
       <c r="F52" s="8" t="s">
         <v>13</v>
       </c>
@@ -3442,11 +3469,11 @@
       <c r="J52" s="1"/>
     </row>
     <row r="53" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="31"/>
-      <c r="B53" s="33"/>
-      <c r="C53" s="33"/>
-      <c r="D53" s="33"/>
-      <c r="E53" s="33"/>
+      <c r="A53" s="21"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
       <c r="F53" s="8">
         <v>1</v>
       </c>
@@ -3462,11 +3489,11 @@
       <c r="J53" s="1"/>
     </row>
     <row r="54" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="31"/>
-      <c r="B54" s="34"/>
-      <c r="C54" s="34"/>
-      <c r="D54" s="34"/>
-      <c r="E54" s="34"/>
+      <c r="A54" s="21"/>
+      <c r="B54" s="19"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="19"/>
       <c r="F54" s="9">
         <v>45047</v>
       </c>
@@ -3482,17 +3509,17 @@
       <c r="J54" s="1"/>
     </row>
     <row r="55" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="31"/>
-      <c r="B55" s="32">
+      <c r="A55" s="21"/>
+      <c r="B55" s="17">
         <v>71</v>
       </c>
-      <c r="C55" s="32">
+      <c r="C55" s="17">
         <v>10</v>
       </c>
-      <c r="D55" s="32" t="s">
+      <c r="D55" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E55" s="32" t="s">
+      <c r="E55" s="17" t="s">
         <v>44</v>
       </c>
       <c r="F55" s="8" t="s">
@@ -3510,11 +3537,11 @@
       <c r="J55" s="1"/>
     </row>
     <row r="56" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="31"/>
-      <c r="B56" s="33"/>
-      <c r="C56" s="33"/>
-      <c r="D56" s="33"/>
-      <c r="E56" s="33"/>
+      <c r="A56" s="21"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
       <c r="F56" s="8" t="s">
         <v>13</v>
       </c>
@@ -3530,11 +3557,11 @@
       <c r="J56" s="1"/>
     </row>
     <row r="57" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="31"/>
-      <c r="B57" s="33"/>
-      <c r="C57" s="33"/>
-      <c r="D57" s="33"/>
-      <c r="E57" s="33"/>
+      <c r="A57" s="21"/>
+      <c r="B57" s="18"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
       <c r="F57" s="8">
         <v>1</v>
       </c>
@@ -3550,11 +3577,11 @@
       <c r="J57" s="1"/>
     </row>
     <row r="58" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="31"/>
-      <c r="B58" s="34"/>
-      <c r="C58" s="34"/>
-      <c r="D58" s="34"/>
-      <c r="E58" s="34"/>
+      <c r="A58" s="21"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="19"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="19"/>
       <c r="F58" s="9">
         <v>45047</v>
       </c>
@@ -3570,17 +3597,17 @@
       <c r="J58" s="1"/>
     </row>
     <row r="59" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="31"/>
-      <c r="B59" s="32">
+      <c r="A59" s="21"/>
+      <c r="B59" s="17">
         <v>71</v>
       </c>
-      <c r="C59" s="32">
+      <c r="C59" s="17">
         <v>11</v>
       </c>
-      <c r="D59" s="32" t="s">
+      <c r="D59" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E59" s="32" t="s">
+      <c r="E59" s="17" t="s">
         <v>44</v>
       </c>
       <c r="F59" s="8" t="s">
@@ -3598,11 +3625,11 @@
       <c r="J59" s="1"/>
     </row>
     <row r="60" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="31"/>
-      <c r="B60" s="33"/>
-      <c r="C60" s="33"/>
-      <c r="D60" s="33"/>
-      <c r="E60" s="33"/>
+      <c r="A60" s="21"/>
+      <c r="B60" s="18"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
       <c r="F60" s="8" t="s">
         <v>13</v>
       </c>
@@ -3618,11 +3645,11 @@
       <c r="J60" s="1"/>
     </row>
     <row r="61" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="31"/>
-      <c r="B61" s="33"/>
-      <c r="C61" s="33"/>
-      <c r="D61" s="33"/>
-      <c r="E61" s="33"/>
+      <c r="A61" s="21"/>
+      <c r="B61" s="18"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
       <c r="F61" s="8">
         <v>1</v>
       </c>
@@ -3638,11 +3665,11 @@
       <c r="J61" s="1"/>
     </row>
     <row r="62" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="31"/>
-      <c r="B62" s="34"/>
-      <c r="C62" s="34"/>
-      <c r="D62" s="34"/>
-      <c r="E62" s="34"/>
+      <c r="A62" s="21"/>
+      <c r="B62" s="19"/>
+      <c r="C62" s="19"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="19"/>
       <c r="F62" s="9">
         <v>45047</v>
       </c>
@@ -3658,17 +3685,17 @@
       <c r="J62" s="1"/>
     </row>
     <row r="63" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="31"/>
-      <c r="B63" s="32">
+      <c r="A63" s="21"/>
+      <c r="B63" s="17">
         <v>71</v>
       </c>
-      <c r="C63" s="32">
+      <c r="C63" s="17">
         <v>12</v>
       </c>
-      <c r="D63" s="32" t="s">
+      <c r="D63" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E63" s="32" t="s">
+      <c r="E63" s="17" t="s">
         <v>44</v>
       </c>
       <c r="F63" s="8" t="s">
@@ -3686,11 +3713,11 @@
       <c r="J63" s="1"/>
     </row>
     <row r="64" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="31"/>
-      <c r="B64" s="33"/>
-      <c r="C64" s="33"/>
-      <c r="D64" s="33"/>
-      <c r="E64" s="33"/>
+      <c r="A64" s="21"/>
+      <c r="B64" s="18"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
       <c r="F64" s="8" t="s">
         <v>13</v>
       </c>
@@ -3706,11 +3733,11 @@
       <c r="J64" s="1"/>
     </row>
     <row r="65" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="31"/>
-      <c r="B65" s="33"/>
-      <c r="C65" s="33"/>
-      <c r="D65" s="33"/>
-      <c r="E65" s="33"/>
+      <c r="A65" s="21"/>
+      <c r="B65" s="18"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
       <c r="F65" s="8">
         <v>1</v>
       </c>
@@ -3726,11 +3753,11 @@
       <c r="J65" s="1"/>
     </row>
     <row r="66" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="31"/>
-      <c r="B66" s="34"/>
-      <c r="C66" s="34"/>
-      <c r="D66" s="34"/>
-      <c r="E66" s="34"/>
+      <c r="A66" s="21"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="19"/>
       <c r="F66" s="9">
         <v>45047</v>
       </c>
@@ -3746,7 +3773,7 @@
       <c r="J66" s="1"/>
     </row>
     <row r="67" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="31"/>
+      <c r="A67" s="21"/>
       <c r="B67" s="8">
         <v>65</v>
       </c>
@@ -3774,7 +3801,7 @@
       <c r="J67" s="1"/>
     </row>
     <row r="68" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="31"/>
+      <c r="A68" s="21"/>
       <c r="B68" s="8">
         <v>75</v>
       </c>
@@ -3802,7 +3829,7 @@
       <c r="J68" s="1"/>
     </row>
     <row r="69" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="31"/>
+      <c r="A69" s="21"/>
       <c r="B69" s="8">
         <v>85</v>
       </c>
@@ -3830,7 +3857,7 @@
       <c r="J69" s="1"/>
     </row>
     <row r="70" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="31"/>
+      <c r="A70" s="21"/>
       <c r="B70" s="8">
         <v>70</v>
       </c>
@@ -3858,7 +3885,7 @@
       <c r="J70" s="1"/>
     </row>
     <row r="71" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="31"/>
+      <c r="A71" s="21"/>
       <c r="B71" s="8">
         <v>70</v>
       </c>
@@ -3886,7 +3913,7 @@
       <c r="J71" s="1"/>
     </row>
     <row r="72" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="31"/>
+      <c r="A72" s="21"/>
       <c r="B72" s="8">
         <v>70</v>
       </c>
@@ -3914,7 +3941,7 @@
       <c r="J72" s="1"/>
     </row>
     <row r="73" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="31"/>
+      <c r="A73" s="21"/>
       <c r="B73" s="8">
         <v>70</v>
       </c>
@@ -3942,7 +3969,7 @@
       <c r="J73" s="1"/>
     </row>
     <row r="74" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="27"/>
+      <c r="A74" s="22"/>
       <c r="B74" s="8">
         <v>80</v>
       </c>
@@ -3971,15 +3998,23 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="B63:B66"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="D63:D66"/>
-    <mergeCell ref="E63:E66"/>
-    <mergeCell ref="E55:E58"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="C59:C62"/>
-    <mergeCell ref="D59:D62"/>
-    <mergeCell ref="E59:E62"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:H2"/>
+    <mergeCell ref="I1:I3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="A23:A38"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A22"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="J23:J24"/>
     <mergeCell ref="A39:A74"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:E15"/>
@@ -3996,23 +4031,15 @@
     <mergeCell ref="B55:B58"/>
     <mergeCell ref="C55:C58"/>
     <mergeCell ref="D55:D58"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="A23:A38"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A22"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="G1:H2"/>
-    <mergeCell ref="I1:I3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="D63:D66"/>
+    <mergeCell ref="E63:E66"/>
+    <mergeCell ref="E55:E58"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="C59:C62"/>
+    <mergeCell ref="D59:D62"/>
+    <mergeCell ref="E59:E62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4022,7 +4049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D34E186-66AB-074A-8BC0-88403B846A52}">
   <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A48" workbookViewId="0">
       <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
@@ -6022,8 +6049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE9A2CE1-3841-0A4B-90A2-869D7C06042C}">
   <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView zoomScale="98" workbookViewId="0">
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6066,7 +6093,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="16" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="13">
@@ -6095,7 +6122,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="16" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="13">
@@ -6124,7 +6151,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="16" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="13">
@@ -6153,7 +6180,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="16" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="13">
@@ -6182,7 +6209,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="13">
@@ -6211,7 +6238,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="13">
@@ -6240,7 +6267,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="13">
@@ -6269,7 +6296,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="13">
@@ -6298,7 +6325,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="13">
@@ -6327,7 +6354,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="13">
@@ -6356,7 +6383,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="13">
@@ -6385,7 +6412,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="13">
@@ -6414,7 +6441,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="13">
@@ -6443,7 +6470,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="13">
@@ -6472,7 +6499,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="13">
@@ -6501,7 +6528,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="13">
@@ -6530,7 +6557,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="13">
@@ -6559,7 +6586,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="13">
@@ -6588,7 +6615,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="13">
@@ -6617,7 +6644,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="13">
@@ -6646,7 +6673,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B22" s="13">
@@ -6673,7 +6700,7 @@
       <c r="I22" s="13"/>
     </row>
     <row r="23" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B23" s="13">
@@ -6702,7 +6729,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B24" s="13">
@@ -6731,7 +6758,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B25" s="13">
@@ -6760,7 +6787,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B26" s="13">
@@ -6789,7 +6816,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B27" s="13">
@@ -6818,7 +6845,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B28" s="13">
@@ -6847,7 +6874,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B29" s="13">
@@ -6876,7 +6903,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B30" s="13">
@@ -6905,7 +6932,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B31" s="13">
@@ -6934,7 +6961,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B32" s="13">
@@ -6963,7 +6990,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A33" s="35" t="s">
+      <c r="A33" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B33" s="13">
@@ -6992,7 +7019,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A34" s="35" t="s">
+      <c r="A34" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B34" s="13">
@@ -7021,7 +7048,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="13">
@@ -7050,7 +7077,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A36" s="35" t="s">
+      <c r="A36" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B36" s="13">
@@ -7079,7 +7106,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B37" s="13">
@@ -7108,7 +7135,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A38" s="35" t="s">
+      <c r="A38" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B38" s="13">
@@ -7137,7 +7164,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A39" s="35" t="s">
+      <c r="A39" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B39" s="13">
@@ -7166,7 +7193,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="35" t="s">
+      <c r="A40" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B40" s="13">
@@ -7195,7 +7222,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B41" s="13">
@@ -7224,7 +7251,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A42" s="35" t="s">
+      <c r="A42" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B42" s="13">
@@ -7253,7 +7280,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A43" s="35" t="s">
+      <c r="A43" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B43" s="13">
@@ -7282,7 +7309,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A44" s="35" t="s">
+      <c r="A44" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B44" s="13">
@@ -7311,7 +7338,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B45" s="13">
@@ -7340,7 +7367,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A46" s="35" t="s">
+      <c r="A46" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B46" s="13">
@@ -7369,7 +7396,7 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A47" s="35" t="s">
+      <c r="A47" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B47" s="13">
@@ -7398,7 +7425,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A48" s="35" t="s">
+      <c r="A48" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B48" s="13">
@@ -7427,7 +7454,7 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A49" s="35" t="s">
+      <c r="A49" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B49" s="13">
@@ -7456,7 +7483,7 @@
       </c>
     </row>
     <row r="50" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A50" s="35" t="s">
+      <c r="A50" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B50" s="13">
@@ -7485,7 +7512,7 @@
       </c>
     </row>
     <row r="51" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A51" s="35" t="s">
+      <c r="A51" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B51" s="13">
@@ -7514,7 +7541,7 @@
       </c>
     </row>
     <row r="52" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A52" s="35" t="s">
+      <c r="A52" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B52" s="13">
@@ -7543,7 +7570,7 @@
       </c>
     </row>
     <row r="53" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A53" s="35" t="s">
+      <c r="A53" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B53" s="13">
@@ -7572,7 +7599,7 @@
       </c>
     </row>
     <row r="54" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A54" s="35" t="s">
+      <c r="A54" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B54" s="13">
@@ -7601,7 +7628,7 @@
       </c>
     </row>
     <row r="55" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A55" s="35" t="s">
+      <c r="A55" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B55" s="13">
@@ -7630,7 +7657,7 @@
       </c>
     </row>
     <row r="56" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A56" s="35" t="s">
+      <c r="A56" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B56" s="13">
@@ -7659,7 +7686,7 @@
       </c>
     </row>
     <row r="57" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A57" s="35" t="s">
+      <c r="A57" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B57" s="13">
@@ -7688,7 +7715,7 @@
       </c>
     </row>
     <row r="58" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A58" s="35" t="s">
+      <c r="A58" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B58" s="13">
@@ -7717,7 +7744,7 @@
       </c>
     </row>
     <row r="59" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A59" s="35" t="s">
+      <c r="A59" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B59" s="13">
@@ -7746,7 +7773,7 @@
       </c>
     </row>
     <row r="60" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A60" s="35" t="s">
+      <c r="A60" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B60" s="13">
@@ -7775,7 +7802,7 @@
       </c>
     </row>
     <row r="61" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A61" s="35" t="s">
+      <c r="A61" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B61" s="13">
@@ -7804,7 +7831,7 @@
       </c>
     </row>
     <row r="62" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A62" s="35" t="s">
+      <c r="A62" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B62" s="13">
@@ -7833,7 +7860,7 @@
       </c>
     </row>
     <row r="63" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A63" s="35" t="s">
+      <c r="A63" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B63" s="13">
@@ -7862,7 +7889,7 @@
       </c>
     </row>
     <row r="64" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A64" s="35" t="s">
+      <c r="A64" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B64" s="13">
@@ -7891,7 +7918,7 @@
       </c>
     </row>
     <row r="65" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A65" s="35" t="s">
+      <c r="A65" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B65" s="13">
@@ -7920,7 +7947,7 @@
       </c>
     </row>
     <row r="66" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A66" s="35" t="s">
+      <c r="A66" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B66" s="13">
@@ -7949,7 +7976,7 @@
       </c>
     </row>
     <row r="67" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A67" s="35" t="s">
+      <c r="A67" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B67" s="13">
@@ -7978,7 +8005,7 @@
       </c>
     </row>
     <row r="68" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A68" s="35" t="s">
+      <c r="A68" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B68" s="13">
@@ -8007,7 +8034,7 @@
       </c>
     </row>
     <row r="69" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A69" s="35" t="s">
+      <c r="A69" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B69" s="13">
@@ -8036,7 +8063,7 @@
       </c>
     </row>
     <row r="70" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A70" s="35" t="s">
+      <c r="A70" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B70" s="13">
@@ -8065,7 +8092,7 @@
       </c>
     </row>
     <row r="71" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A71" s="35" t="s">
+      <c r="A71" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B71" s="13">
@@ -8094,7 +8121,7 @@
       </c>
     </row>
     <row r="72" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A72" s="35" t="s">
+      <c r="A72" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B72" s="13">
@@ -8123,7 +8150,7 @@
       </c>
     </row>
     <row r="73" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A73" s="35" t="s">
+      <c r="A73" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B73" s="13">
@@ -8152,7 +8179,7 @@
       </c>
     </row>
     <row r="74" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A74" s="35" t="s">
+      <c r="A74" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B74" s="13">
@@ -8181,7 +8208,7 @@
       </c>
     </row>
     <row r="75" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A75" s="35" t="s">
+      <c r="A75" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B75" s="13">
@@ -8210,7 +8237,7 @@
       </c>
     </row>
     <row r="76" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A76" s="35" t="s">
+      <c r="A76" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B76" s="13">
@@ -8239,7 +8266,7 @@
       </c>
     </row>
     <row r="77" spans="1:9" ht="19" x14ac:dyDescent="0.2">
-      <c r="A77" s="35" t="s">
+      <c r="A77" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B77" s="13">
@@ -8274,4 +8301,1723 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4479104-9740-3841-AB70-E3C9415F1FB2}">
+  <dimension ref="A1:H65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="38.83203125" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>45</v>
+      </c>
+      <c r="C2">
+        <v>60</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>0.5</v>
+      </c>
+      <c r="F2">
+        <v>618.5</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="H2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>80</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>0.5</v>
+      </c>
+      <c r="F3">
+        <v>978.1</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
+      </c>
+      <c r="H3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>45</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>0.5</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>45</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>0.47</v>
+      </c>
+      <c r="F5">
+        <v>2.6280000000000001</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>50</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>0.2</v>
+      </c>
+      <c r="F6">
+        <v>1712</v>
+      </c>
+      <c r="G6">
+        <v>100</v>
+      </c>
+      <c r="H6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>0.2</v>
+      </c>
+      <c r="F7">
+        <v>889.6</v>
+      </c>
+      <c r="G7">
+        <v>100</v>
+      </c>
+      <c r="H7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>80</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>0.2</v>
+      </c>
+      <c r="F8">
+        <v>1.7</v>
+      </c>
+      <c r="G8">
+        <v>100</v>
+      </c>
+      <c r="H8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>45</v>
+      </c>
+      <c r="C9">
+        <v>60</v>
+      </c>
+      <c r="D9">
+        <v>0.3</v>
+      </c>
+      <c r="E9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F9">
+        <v>2000</v>
+      </c>
+      <c r="G9">
+        <v>100</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>60</v>
+      </c>
+      <c r="C10">
+        <v>60</v>
+      </c>
+      <c r="D10">
+        <v>0.3</v>
+      </c>
+      <c r="E10">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F10">
+        <v>2000</v>
+      </c>
+      <c r="G10">
+        <v>100</v>
+      </c>
+      <c r="H10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <v>60</v>
+      </c>
+      <c r="C11">
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <v>0.3</v>
+      </c>
+      <c r="E11">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F11">
+        <v>2000</v>
+      </c>
+      <c r="G11">
+        <v>100</v>
+      </c>
+      <c r="H11">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>45</v>
+      </c>
+      <c r="C12">
+        <v>130</v>
+      </c>
+      <c r="D12">
+        <v>0.1</v>
+      </c>
+      <c r="E12">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F12">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="G12">
+        <v>99.5</v>
+      </c>
+      <c r="H12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>45</v>
+      </c>
+      <c r="C13">
+        <v>130</v>
+      </c>
+      <c r="D13">
+        <v>0.1</v>
+      </c>
+      <c r="E13">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F13">
+        <v>21.3</v>
+      </c>
+      <c r="G13">
+        <v>0.5</v>
+      </c>
+      <c r="H13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>45</v>
+      </c>
+      <c r="C14">
+        <v>83</v>
+      </c>
+      <c r="D14">
+        <v>0.26</v>
+      </c>
+      <c r="E14">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F14">
+        <v>2000</v>
+      </c>
+      <c r="G14">
+        <v>100</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>25</v>
+      </c>
+      <c r="C15">
+        <v>61</v>
+      </c>
+      <c r="D15">
+        <v>0.26</v>
+      </c>
+      <c r="E15">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F15">
+        <v>2000</v>
+      </c>
+      <c r="G15">
+        <v>100</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16">
+        <v>45</v>
+      </c>
+      <c r="C16">
+        <v>56</v>
+      </c>
+      <c r="D16">
+        <v>0.26</v>
+      </c>
+      <c r="E16">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F16">
+        <v>2000</v>
+      </c>
+      <c r="G16">
+        <v>100</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>25</v>
+      </c>
+      <c r="C17">
+        <v>60</v>
+      </c>
+      <c r="D17">
+        <v>0.53</v>
+      </c>
+      <c r="E17">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F17">
+        <v>832.4</v>
+      </c>
+      <c r="G17">
+        <v>100</v>
+      </c>
+      <c r="H17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <v>58</v>
+      </c>
+      <c r="D18">
+        <v>0.53</v>
+      </c>
+      <c r="E18">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F18">
+        <v>716.2</v>
+      </c>
+      <c r="G18">
+        <v>100</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>80</v>
+      </c>
+      <c r="C19">
+        <v>60</v>
+      </c>
+      <c r="D19">
+        <v>0.1</v>
+      </c>
+      <c r="E19">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F19">
+        <v>2000</v>
+      </c>
+      <c r="G19">
+        <v>100</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>45</v>
+      </c>
+      <c r="C20">
+        <v>130</v>
+      </c>
+      <c r="D20">
+        <v>0.1</v>
+      </c>
+      <c r="E20">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F20">
+        <v>5.4</v>
+      </c>
+      <c r="G20">
+        <v>100</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21">
+        <v>50</v>
+      </c>
+      <c r="C21">
+        <v>30</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <v>0.3</v>
+      </c>
+      <c r="F21">
+        <v>2159</v>
+      </c>
+      <c r="G21">
+        <v>41.6</v>
+      </c>
+      <c r="H21">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22">
+        <v>50</v>
+      </c>
+      <c r="C22">
+        <v>30</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <v>0.3</v>
+      </c>
+      <c r="F22">
+        <v>487.2</v>
+      </c>
+      <c r="G22">
+        <v>58.4</v>
+      </c>
+      <c r="H22">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23">
+        <v>80</v>
+      </c>
+      <c r="C23">
+        <v>20</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <v>0.3</v>
+      </c>
+      <c r="F23">
+        <v>1021</v>
+      </c>
+      <c r="G23">
+        <v>100</v>
+      </c>
+      <c r="H23">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24">
+        <v>45</v>
+      </c>
+      <c r="C24">
+        <v>60</v>
+      </c>
+      <c r="D24">
+        <v>0.3</v>
+      </c>
+      <c r="E24">
+        <v>0.35</v>
+      </c>
+      <c r="F24">
+        <v>2000</v>
+      </c>
+      <c r="G24">
+        <v>100</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A25" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25">
+        <v>60</v>
+      </c>
+      <c r="C25">
+        <v>60</v>
+      </c>
+      <c r="D25">
+        <v>0.3</v>
+      </c>
+      <c r="E25">
+        <v>0.35</v>
+      </c>
+      <c r="F25">
+        <v>2000</v>
+      </c>
+      <c r="G25">
+        <v>100</v>
+      </c>
+      <c r="H25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A26" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26">
+        <v>60</v>
+      </c>
+      <c r="C26">
+        <v>30</v>
+      </c>
+      <c r="D26">
+        <v>0.3</v>
+      </c>
+      <c r="E26">
+        <v>0.35</v>
+      </c>
+      <c r="F26">
+        <v>2000</v>
+      </c>
+      <c r="G26">
+        <v>100</v>
+      </c>
+      <c r="H26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A27" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27">
+        <v>60</v>
+      </c>
+      <c r="C27">
+        <v>60</v>
+      </c>
+      <c r="D27">
+        <v>0.3</v>
+      </c>
+      <c r="E27">
+        <v>0.17</v>
+      </c>
+      <c r="F27">
+        <v>2000</v>
+      </c>
+      <c r="G27">
+        <v>100</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A28" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28">
+        <v>80</v>
+      </c>
+      <c r="C28">
+        <v>20</v>
+      </c>
+      <c r="D28">
+        <v>0.3</v>
+      </c>
+      <c r="E28">
+        <v>0.17</v>
+      </c>
+      <c r="F28">
+        <v>2000</v>
+      </c>
+      <c r="G28">
+        <v>100</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A29" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29">
+        <v>60</v>
+      </c>
+      <c r="C29">
+        <v>40</v>
+      </c>
+      <c r="D29">
+        <v>0.3</v>
+      </c>
+      <c r="E29">
+        <v>0.17</v>
+      </c>
+      <c r="F29">
+        <v>2000</v>
+      </c>
+      <c r="G29">
+        <v>100</v>
+      </c>
+      <c r="H29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A30" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30">
+        <v>45</v>
+      </c>
+      <c r="C30">
+        <v>70</v>
+      </c>
+      <c r="D30">
+        <v>0.8</v>
+      </c>
+      <c r="E30">
+        <v>0.17</v>
+      </c>
+      <c r="F30">
+        <v>2000</v>
+      </c>
+      <c r="G30">
+        <v>100</v>
+      </c>
+      <c r="H30">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A31" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31">
+        <v>20</v>
+      </c>
+      <c r="C31">
+        <v>50</v>
+      </c>
+      <c r="D31">
+        <v>1.58</v>
+      </c>
+      <c r="E31">
+        <v>0.15</v>
+      </c>
+      <c r="F31">
+        <v>2000</v>
+      </c>
+      <c r="G31">
+        <v>100</v>
+      </c>
+      <c r="H31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A32" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32">
+        <v>20</v>
+      </c>
+      <c r="C32">
+        <v>80</v>
+      </c>
+      <c r="D32">
+        <v>1.58</v>
+      </c>
+      <c r="E32">
+        <v>0.15</v>
+      </c>
+      <c r="F32">
+        <v>2000</v>
+      </c>
+      <c r="G32">
+        <v>100</v>
+      </c>
+      <c r="H32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A33" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33">
+        <v>20</v>
+      </c>
+      <c r="C33">
+        <v>60</v>
+      </c>
+      <c r="D33">
+        <v>2.38</v>
+      </c>
+      <c r="E33">
+        <v>0.15</v>
+      </c>
+      <c r="F33">
+        <v>2000</v>
+      </c>
+      <c r="G33">
+        <v>100</v>
+      </c>
+      <c r="H33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A34" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <v>25</v>
+      </c>
+      <c r="C34">
+        <v>60</v>
+      </c>
+      <c r="D34">
+        <v>2.38</v>
+      </c>
+      <c r="E34">
+        <v>0.15</v>
+      </c>
+      <c r="F34">
+        <v>2000</v>
+      </c>
+      <c r="G34">
+        <v>100</v>
+      </c>
+      <c r="H34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A35" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>45</v>
+      </c>
+      <c r="C35">
+        <v>20</v>
+      </c>
+      <c r="D35">
+        <v>4</v>
+      </c>
+      <c r="E35">
+        <v>0.47</v>
+      </c>
+      <c r="F35">
+        <v>0.7</v>
+      </c>
+      <c r="G35">
+        <v>100</v>
+      </c>
+      <c r="H35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A36" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>45</v>
+      </c>
+      <c r="C36">
+        <v>20</v>
+      </c>
+      <c r="D36">
+        <v>4</v>
+      </c>
+      <c r="E36">
+        <v>0.47</v>
+      </c>
+      <c r="F36">
+        <v>2.6280000000000001</v>
+      </c>
+      <c r="G36">
+        <v>100</v>
+      </c>
+      <c r="H36">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A37" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37">
+        <v>45</v>
+      </c>
+      <c r="C37">
+        <v>20</v>
+      </c>
+      <c r="D37">
+        <v>4</v>
+      </c>
+      <c r="E37">
+        <v>0.22</v>
+      </c>
+      <c r="F37">
+        <v>3096</v>
+      </c>
+      <c r="G37">
+        <v>100</v>
+      </c>
+      <c r="H37">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A38" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38">
+        <v>35</v>
+      </c>
+      <c r="C38">
+        <v>60</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38">
+        <v>0.42</v>
+      </c>
+      <c r="F38">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="G38">
+        <v>100</v>
+      </c>
+      <c r="H38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A39" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39">
+        <v>35</v>
+      </c>
+      <c r="C39">
+        <v>20</v>
+      </c>
+      <c r="D39">
+        <v>3</v>
+      </c>
+      <c r="E39">
+        <v>0.4</v>
+      </c>
+      <c r="F39">
+        <v>1.71</v>
+      </c>
+      <c r="G39">
+        <v>100</v>
+      </c>
+      <c r="H39">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A40" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40">
+        <v>35</v>
+      </c>
+      <c r="C40">
+        <v>90</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40">
+        <v>0.38</v>
+      </c>
+      <c r="F40">
+        <v>3.46</v>
+      </c>
+      <c r="G40">
+        <v>100</v>
+      </c>
+      <c r="H40">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A41" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41">
+        <v>80</v>
+      </c>
+      <c r="C41">
+        <v>8</v>
+      </c>
+      <c r="D41">
+        <v>0.1</v>
+      </c>
+      <c r="E41">
+        <v>0.6</v>
+      </c>
+      <c r="F41">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="G41">
+        <v>100</v>
+      </c>
+      <c r="H41">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A42" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42">
+        <v>85</v>
+      </c>
+      <c r="C42">
+        <v>9</v>
+      </c>
+      <c r="D42">
+        <v>0.1</v>
+      </c>
+      <c r="E42">
+        <v>0.6</v>
+      </c>
+      <c r="F42">
+        <v>2.1</v>
+      </c>
+      <c r="G42">
+        <v>100</v>
+      </c>
+      <c r="H42">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A43" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43">
+        <v>80</v>
+      </c>
+      <c r="C43">
+        <v>9</v>
+      </c>
+      <c r="D43">
+        <v>0.1</v>
+      </c>
+      <c r="E43">
+        <v>0.6</v>
+      </c>
+      <c r="F43">
+        <v>2.4220000000000002</v>
+      </c>
+      <c r="G43">
+        <v>100</v>
+      </c>
+      <c r="H43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A44" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>80</v>
+      </c>
+      <c r="C44">
+        <v>10</v>
+      </c>
+      <c r="D44">
+        <v>0.1</v>
+      </c>
+      <c r="E44">
+        <v>0.6</v>
+      </c>
+      <c r="F44">
+        <v>2.101</v>
+      </c>
+      <c r="G44">
+        <v>100</v>
+      </c>
+      <c r="H44">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A45" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>80</v>
+      </c>
+      <c r="C45">
+        <v>11</v>
+      </c>
+      <c r="D45">
+        <v>0.1</v>
+      </c>
+      <c r="E45">
+        <v>0.6</v>
+      </c>
+      <c r="F45">
+        <v>2.2690000000000001</v>
+      </c>
+      <c r="G45">
+        <v>100</v>
+      </c>
+      <c r="H45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A46" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46">
+        <v>80</v>
+      </c>
+      <c r="C46">
+        <v>12</v>
+      </c>
+      <c r="D46">
+        <v>0.1</v>
+      </c>
+      <c r="E46">
+        <v>0.6</v>
+      </c>
+      <c r="F46">
+        <v>1.7529999999999999</v>
+      </c>
+      <c r="G46">
+        <v>96.6</v>
+      </c>
+      <c r="H46">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A47" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47">
+        <v>85</v>
+      </c>
+      <c r="C47">
+        <v>11</v>
+      </c>
+      <c r="D47">
+        <v>0.1</v>
+      </c>
+      <c r="E47">
+        <v>0.6</v>
+      </c>
+      <c r="F47">
+        <v>1.3320000000000001</v>
+      </c>
+      <c r="G47">
+        <v>98.8</v>
+      </c>
+      <c r="H47">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A48" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B48">
+        <v>88</v>
+      </c>
+      <c r="C48">
+        <v>9</v>
+      </c>
+      <c r="D48">
+        <v>0.1</v>
+      </c>
+      <c r="E48">
+        <v>0.6</v>
+      </c>
+      <c r="F48">
+        <v>2.496</v>
+      </c>
+      <c r="G48">
+        <v>100</v>
+      </c>
+      <c r="H48">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A49" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49">
+        <v>88</v>
+      </c>
+      <c r="C49">
+        <v>10</v>
+      </c>
+      <c r="D49">
+        <v>0.1</v>
+      </c>
+      <c r="E49">
+        <v>0.6</v>
+      </c>
+      <c r="F49">
+        <v>2.3069999999999999</v>
+      </c>
+      <c r="G49">
+        <v>99.3</v>
+      </c>
+      <c r="H49">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A50" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50">
+        <v>89</v>
+      </c>
+      <c r="C50">
+        <v>9</v>
+      </c>
+      <c r="D50">
+        <v>0.1</v>
+      </c>
+      <c r="E50">
+        <v>0.6</v>
+      </c>
+      <c r="F50">
+        <v>1.8779999999999999</v>
+      </c>
+      <c r="G50">
+        <v>100</v>
+      </c>
+      <c r="H50">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A51" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B51">
+        <v>89</v>
+      </c>
+      <c r="C51">
+        <v>10</v>
+      </c>
+      <c r="D51">
+        <v>0.1</v>
+      </c>
+      <c r="E51">
+        <v>0.6</v>
+      </c>
+      <c r="F51">
+        <v>2.069</v>
+      </c>
+      <c r="G51">
+        <v>100</v>
+      </c>
+      <c r="H51">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A52" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B52">
+        <v>93</v>
+      </c>
+      <c r="C52">
+        <v>11</v>
+      </c>
+      <c r="D52">
+        <v>0.1</v>
+      </c>
+      <c r="E52">
+        <v>0.6</v>
+      </c>
+      <c r="F52">
+        <v>2.7629999999999999</v>
+      </c>
+      <c r="G52">
+        <v>100</v>
+      </c>
+      <c r="H52">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A53" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B53">
+        <v>93</v>
+      </c>
+      <c r="C53">
+        <v>12</v>
+      </c>
+      <c r="D53">
+        <v>0.1</v>
+      </c>
+      <c r="E53">
+        <v>0.6</v>
+      </c>
+      <c r="F53">
+        <v>3.2189999999999999</v>
+      </c>
+      <c r="G53">
+        <v>99.7</v>
+      </c>
+      <c r="H53">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A54" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B54">
+        <v>71</v>
+      </c>
+      <c r="C54">
+        <v>9</v>
+      </c>
+      <c r="D54">
+        <v>0.1</v>
+      </c>
+      <c r="E54">
+        <v>0.6</v>
+      </c>
+      <c r="F54">
+        <v>1.893</v>
+      </c>
+      <c r="G54">
+        <v>100</v>
+      </c>
+      <c r="H54">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A55" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B55">
+        <v>71</v>
+      </c>
+      <c r="C55">
+        <v>10</v>
+      </c>
+      <c r="D55">
+        <v>0.1</v>
+      </c>
+      <c r="E55">
+        <v>0.6</v>
+      </c>
+      <c r="F55">
+        <v>1.958</v>
+      </c>
+      <c r="G55">
+        <v>100</v>
+      </c>
+      <c r="H55">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A56" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B56">
+        <v>71</v>
+      </c>
+      <c r="C56">
+        <v>11</v>
+      </c>
+      <c r="D56">
+        <v>0.1</v>
+      </c>
+      <c r="E56">
+        <v>0.6</v>
+      </c>
+      <c r="F56">
+        <v>2.1760000000000002</v>
+      </c>
+      <c r="G56">
+        <v>100</v>
+      </c>
+      <c r="H56">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A57" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B57">
+        <v>71</v>
+      </c>
+      <c r="C57">
+        <v>12</v>
+      </c>
+      <c r="D57">
+        <v>0.1</v>
+      </c>
+      <c r="E57">
+        <v>0.6</v>
+      </c>
+      <c r="F57">
+        <v>2.1850000000000001</v>
+      </c>
+      <c r="G57">
+        <v>100</v>
+      </c>
+      <c r="H57">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A58" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B58">
+        <v>65</v>
+      </c>
+      <c r="C58">
+        <v>12</v>
+      </c>
+      <c r="D58">
+        <v>0.1</v>
+      </c>
+      <c r="E58">
+        <v>0.6</v>
+      </c>
+      <c r="F58">
+        <v>1.377</v>
+      </c>
+      <c r="G58">
+        <v>97.5</v>
+      </c>
+      <c r="H58">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A59" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B59">
+        <v>75</v>
+      </c>
+      <c r="C59">
+        <v>12</v>
+      </c>
+      <c r="D59">
+        <v>0.1</v>
+      </c>
+      <c r="E59">
+        <v>0.6</v>
+      </c>
+      <c r="F59">
+        <v>3.3039999999999998</v>
+      </c>
+      <c r="G59">
+        <v>100</v>
+      </c>
+      <c r="H59">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A60" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B60">
+        <v>85</v>
+      </c>
+      <c r="C60">
+        <v>12</v>
+      </c>
+      <c r="D60">
+        <v>0.1</v>
+      </c>
+      <c r="E60">
+        <v>0.6</v>
+      </c>
+      <c r="F60">
+        <v>2000</v>
+      </c>
+      <c r="G60">
+        <v>100</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A61" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B61">
+        <v>70</v>
+      </c>
+      <c r="C61">
+        <v>12</v>
+      </c>
+      <c r="D61">
+        <v>0.1</v>
+      </c>
+      <c r="E61">
+        <v>0.62</v>
+      </c>
+      <c r="F61">
+        <v>2.9</v>
+      </c>
+      <c r="G61">
+        <v>99.5</v>
+      </c>
+      <c r="H61">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A62" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B62">
+        <v>70</v>
+      </c>
+      <c r="C62">
+        <v>12</v>
+      </c>
+      <c r="D62">
+        <v>0.1</v>
+      </c>
+      <c r="E62">
+        <v>0.59</v>
+      </c>
+      <c r="F62">
+        <v>1.901</v>
+      </c>
+      <c r="G62">
+        <v>100</v>
+      </c>
+      <c r="H62">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A63" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B63">
+        <v>70</v>
+      </c>
+      <c r="C63">
+        <v>12</v>
+      </c>
+      <c r="D63">
+        <v>0.1</v>
+      </c>
+      <c r="E63">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F63">
+        <v>2.8410000000000002</v>
+      </c>
+      <c r="G63">
+        <v>100</v>
+      </c>
+      <c r="H63">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A64" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B64">
+        <v>70</v>
+      </c>
+      <c r="C64">
+        <v>12</v>
+      </c>
+      <c r="D64">
+        <v>0.1</v>
+      </c>
+      <c r="E64">
+        <v>0.52</v>
+      </c>
+      <c r="F64">
+        <v>2.1619999999999999</v>
+      </c>
+      <c r="G64">
+        <v>97.8</v>
+      </c>
+      <c r="H64">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A65" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B65">
+        <v>80</v>
+      </c>
+      <c r="C65">
+        <v>8</v>
+      </c>
+      <c r="D65">
+        <v>0.1</v>
+      </c>
+      <c r="E65">
+        <v>0.6</v>
+      </c>
+      <c r="F65">
+        <v>2.1970000000000001</v>
+      </c>
+      <c r="G65">
+        <v>100</v>
+      </c>
+      <c r="H65">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>